<commit_message>
Completed Preliminary Schematic of Version 1.0 of the PFC
</commit_message>
<xml_diff>
--- a/Power Factor Correction/Design Files/UC2855A Calculations (Autosaved).xlsx
+++ b/Power Factor Correction/Design Files/UC2855A Calculations (Autosaved).xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tv\Real Documents\Engineering Projects\Senior-Design-VFD\Power-Factor-Correction\Design Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tv\Real Documents\Engineering Projects\Senior-Design-VFD\Power Factor Correction\Design Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17925" windowHeight="9735"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Power Factor Correction" sheetId="1" r:id="rId1"/>
+    <sheet name="Inductor Design Calculation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="138">
   <si>
     <t>Oscillator</t>
   </si>
@@ -210,9 +211,6 @@
   </si>
   <si>
     <t>Vo(min)</t>
-  </si>
-  <si>
-    <t>The equivalent resonant capacitance is equal to the Coss (output capacitance) plus an additional capcitor in parallelle  with the main power MOSFET</t>
   </si>
   <si>
     <t xml:space="preserve">tZVT </t>
@@ -376,9 +374,6 @@
     <t>Rf</t>
   </si>
   <si>
-    <t>1/(2*PI()*</t>
-  </si>
-  <si>
     <t>Rounded to 180pF</t>
   </si>
   <si>
@@ -395,16 +390,83 @@
   </si>
   <si>
     <t>ESMR451VSN121MP25S</t>
+  </si>
+  <si>
+    <t>Vea</t>
+  </si>
+  <si>
+    <t>GVEA</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>Tv</t>
+  </si>
+  <si>
+    <t>GVEA(for Tv)</t>
+  </si>
+  <si>
+    <t>OVP Enable</t>
+  </si>
+  <si>
+    <t>Top R</t>
+  </si>
+  <si>
+    <t>Bottom R</t>
+  </si>
+  <si>
+    <t>The equivalent resonant capacitance is equal to the Coss (output capacitance) plus an additional capcitor in paralell  with the main power MOSFET</t>
+  </si>
+  <si>
+    <t>Desired Inductance</t>
+  </si>
+  <si>
+    <t>Desired Current Rating</t>
+  </si>
+  <si>
+    <t>ETD39</t>
+  </si>
+  <si>
+    <t>ETD44</t>
+  </si>
+  <si>
+    <t>ETD49</t>
+  </si>
+  <si>
+    <t>ETD54</t>
+  </si>
+  <si>
+    <t>Ae (mm^2)</t>
+  </si>
+  <si>
+    <t>ETD29 0.2mm Gap</t>
+  </si>
+  <si>
+    <t>ETD34 N87  1mm Gap</t>
+  </si>
+  <si>
+    <t>Al (Permiance)</t>
+  </si>
+  <si>
+    <t>N Number of turns</t>
+  </si>
+  <si>
+    <t>Bmax (mT)</t>
+  </si>
+  <si>
+    <t>B  Calculated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
-    <numFmt numFmtId="175" formatCode="0.00000000"/>
-    <numFmt numFmtId="183" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
+    <numFmt numFmtId="179" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="180" formatCode="0.000000000000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -449,12 +511,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="15">
@@ -612,7 +680,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -760,121 +828,126 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4040,10 +4113,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4051,7 +4124,7 @@
     <col min="3" max="4" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
     <col min="12" max="12" width="11.140625" customWidth="1"/>
   </cols>
@@ -4088,14 +4161,14 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="65" t="s">
+      <c r="J3" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
@@ -4119,15 +4192,15 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="72">
+      <c r="B7" s="68">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="68" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
       <c r="G7" t="s">
         <v>1</v>
       </c>
@@ -4136,11 +4209,11 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="83"/>
       <c r="G8" t="s">
         <v>58</v>
       </c>
@@ -4150,11 +4223,11 @@
       </c>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="82"/>
-      <c r="C9" s="82"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
       <c r="G9" s="16" t="s">
         <v>2</v>
       </c>
@@ -4163,22 +4236,22 @@
         <v>1.7857142857142858E-10</v>
       </c>
       <c r="I9" s="16"/>
-      <c r="J9" s="65" t="s">
-        <v>112</v>
-      </c>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="65"/>
-      <c r="O9" s="65"/>
+      <c r="J9" s="79" t="s">
+        <v>110</v>
+      </c>
+      <c r="K9" s="79"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="79"/>
     </row>
     <row r="10" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="47"/>
-      <c r="C10" s="96" t="s">
+      <c r="C10" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="47" t="s">
         <v>67</v>
-      </c>
-      <c r="D10" s="47" t="s">
-        <v>68</v>
       </c>
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
@@ -4187,10 +4260,10 @@
         <v>1000</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J10" s="62" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K10" s="62"/>
       <c r="L10" s="62"/>
@@ -4199,12 +4272,12 @@
       <c r="O10" s="62"/>
     </row>
     <row r="11" spans="2:15" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="96">
+      <c r="B11" s="73">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C11" s="63"/>
+      <c r="C11" s="64"/>
       <c r="D11" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -4223,15 +4296,15 @@
       <c r="O11" s="62"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E12" s="35"/>
       <c r="F12" s="35"/>
       <c r="G12" s="22"/>
-      <c r="H12" s="97">
+      <c r="H12" s="61">
         <f>-1*(H11*10^-12)*H10*LN(1-(2.5/7.5))</f>
         <v>8.9202323783796128E-8</v>
       </c>
@@ -4249,15 +4322,15 @@
       <c r="B13" s="37">
         <v>3</v>
       </c>
-      <c r="C13" s="93" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
+      <c r="C13" s="85" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
@@ -4267,10 +4340,10 @@
     </row>
     <row r="14" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="44" t="s">
         <v>72</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>73</v>
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="50"/>
@@ -4286,11 +4359,11 @@
       <c r="O14" s="17"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="66" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="66" t="s">
-        <v>77</v>
+      <c r="B15" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>76</v>
       </c>
       <c r="D15" s="39"/>
       <c r="E15" s="40"/>
@@ -4300,7 +4373,7 @@
         <v>500</v>
       </c>
       <c r="I15" s="53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J15" s="38"/>
       <c r="K15" s="38"/>
@@ -4310,10 +4383,10 @@
       <c r="O15" s="38"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
       <c r="D16" s="43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E16" s="41"/>
       <c r="F16" s="41"/>
@@ -4323,7 +4396,7 @@
         <v>763675.32368147129</v>
       </c>
       <c r="I16" s="56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J16" s="38"/>
       <c r="K16" s="38"/>
@@ -4334,10 +4407,10 @@
     </row>
     <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="55"/>
@@ -4348,7 +4421,7 @@
         <v>3205.1282051282055</v>
       </c>
       <c r="I17" s="58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J17" s="38"/>
       <c r="K17" s="38"/>
@@ -4358,23 +4431,23 @@
       <c r="O17" s="38"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="66">
+      <c r="B18" s="63">
         <v>3.2</v>
       </c>
-      <c r="C18" s="66" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="69" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" s="69"/>
+      <c r="C18" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" s="66"/>
       <c r="F18" s="48"/>
       <c r="G18" s="19"/>
       <c r="H18" s="34">
         <v>100</v>
       </c>
       <c r="I18" s="54" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J18" s="49"/>
       <c r="K18" s="49"/>
@@ -4384,25 +4457,25 @@
       <c r="O18" s="49"/>
     </row>
     <row r="19" spans="2:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="72" t="s">
-        <v>81</v>
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="68" t="s">
+        <v>80</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H19" s="34">
         <f>1/(H24/H18)</f>
         <v>12.977016495639477</v>
       </c>
       <c r="I19" s="54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J19" s="62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K19" s="62"/>
       <c r="L19" s="62"/>
@@ -4411,9 +4484,9 @@
       <c r="O19" s="62"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="72"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="68"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="19"/>
@@ -4425,7 +4498,7 @@
         <v>10</v>
       </c>
       <c r="J20" s="62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K20" s="62"/>
       <c r="L20" s="62"/>
@@ -4434,21 +4507,21 @@
       <c r="O20" s="62"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
       <c r="D21" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E21" s="40"/>
       <c r="F21" s="40"/>
       <c r="G21" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H21" s="34">
         <v>220000</v>
       </c>
       <c r="I21" s="54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J21" s="38"/>
       <c r="K21" s="38"/>
@@ -4458,50 +4531,50 @@
       <c r="O21" s="38"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
       <c r="D22" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="H22" s="98">
+        <v>83</v>
+      </c>
+      <c r="H22" s="100">
         <f>(3*H27*H18)/(H21*H4*H19)</f>
         <v>3.325238512566868E-11</v>
       </c>
       <c r="I22" s="54" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <v>4.2</v>
       </c>
-      <c r="C23" s="94" t="s">
+      <c r="C23" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="94"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="2:15" ht="53.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="95" t="s">
+      <c r="B24" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="96" t="s">
+      <c r="C24" s="73" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="91"/>
-      <c r="F24" s="91"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
       <c r="G24" s="4" t="s">
         <v>13</v>
       </c>
@@ -4512,23 +4585,23 @@
       <c r="I24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J24" s="90" t="s">
+      <c r="J24" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="90"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="90"/>
-      <c r="N24" s="90"/>
-      <c r="O24" s="90"/>
+      <c r="K24" s="78"/>
+      <c r="L24" s="78"/>
+      <c r="M24" s="78"/>
+      <c r="N24" s="78"/>
+      <c r="O24" s="78"/>
     </row>
     <row r="25" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="70"/>
-      <c r="C25" s="67"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="74"/>
       <c r="D25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
       <c r="G25" s="5" t="s">
         <v>16</v>
       </c>
@@ -4539,21 +4612,21 @@
       <c r="I25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="92" t="s">
+      <c r="J25" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="K25" s="92"/>
-      <c r="L25" s="92"/>
-      <c r="M25" s="92"/>
-      <c r="N25" s="92"/>
-      <c r="O25" s="92"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="82"/>
+      <c r="N25" s="82"/>
+      <c r="O25" s="82"/>
     </row>
     <row r="26" spans="2:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="81"/>
       <c r="G26" s="10" t="s">
         <v>21</v>
       </c>
@@ -4575,8 +4648,8 @@
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="76"/>
       <c r="G27" s="21" t="s">
         <v>23</v>
       </c>
@@ -4587,12 +4660,12 @@
       <c r="I27" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="89"/>
-      <c r="K27" s="89"/>
-      <c r="L27" s="89"/>
-      <c r="M27" s="89"/>
-      <c r="N27" s="89"/>
-      <c r="O27" s="89"/>
+      <c r="J27" s="77"/>
+      <c r="K27" s="77"/>
+      <c r="L27" s="77"/>
+      <c r="M27" s="77"/>
+      <c r="N27" s="77"/>
+      <c r="O27" s="77"/>
     </row>
     <row r="28" spans="2:15" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
@@ -4604,8 +4677,8 @@
       <c r="D28" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
       <c r="G28" s="23" t="s">
         <v>28</v>
       </c>
@@ -4614,75 +4687,75 @@
         <v>5.1083900226757363E-4</v>
       </c>
       <c r="I28" s="25"/>
-      <c r="J28" s="99" t="s">
-        <v>117</v>
-      </c>
-      <c r="K28" s="99"/>
-      <c r="L28" s="99"/>
-      <c r="M28" s="99"/>
-      <c r="N28" s="99"/>
+      <c r="J28" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="67"/>
+      <c r="N28" s="67"/>
     </row>
     <row r="29" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="72" t="s">
+      <c r="B29" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="63" t="s">
+      <c r="C29" s="64" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="85" t="s">
+      <c r="E29" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="85"/>
-      <c r="G29" s="85"/>
-      <c r="H29" s="85"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="87"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="86" t="s">
+      <c r="J29" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="K29" s="86"/>
+      <c r="K29" s="88"/>
       <c r="L29" t="s">
         <v>33</v>
       </c>
-      <c r="M29" s="86" t="s">
+      <c r="M29" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="N29" s="86"/>
+      <c r="N29" s="88"/>
     </row>
     <row r="30" spans="2:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="72"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="79" t="s">
+      <c r="B30" s="68"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="87" t="s">
+      <c r="E30" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87"/>
-      <c r="J30" s="86" t="s">
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="89"/>
+      <c r="J30" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="K30" s="86"/>
+      <c r="K30" s="88"/>
       <c r="L30" t="s">
         <v>33</v>
       </c>
-      <c r="M30" s="86" t="s">
+      <c r="M30" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="N30" s="86"/>
+      <c r="N30" s="88"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="82"/>
-      <c r="C31" s="81"/>
-      <c r="D31" s="80"/>
-      <c r="E31" s="83" t="s">
+      <c r="B31" s="69"/>
+      <c r="C31" s="94"/>
+      <c r="D31" s="93"/>
+      <c r="E31" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="83"/>
+      <c r="F31" s="84"/>
       <c r="G31" s="20" t="s">
         <v>38</v>
       </c>
@@ -4697,28 +4770,28 @@
       <c r="B32" s="27">
         <v>4.3</v>
       </c>
-      <c r="C32" s="77" t="s">
+      <c r="C32" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="77"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="77"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="77"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="90"/>
+      <c r="G32" s="90"/>
+      <c r="H32" s="90"/>
+      <c r="I32" s="90"/>
     </row>
     <row r="33" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="69" t="s">
+      <c r="B33" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="66" t="s">
+      <c r="C33" s="63" t="s">
         <v>42</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="91"/>
       <c r="G33" s="28" t="s">
         <v>47</v>
       </c>
@@ -4729,23 +4802,23 @@
       <c r="I33" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="J33" s="73" t="s">
+      <c r="J33" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="K33" s="73"/>
-      <c r="L33" s="73"/>
-      <c r="M33" s="73"/>
-      <c r="N33" s="73"/>
-      <c r="O33" s="73"/>
+      <c r="K33" s="97"/>
+      <c r="L33" s="97"/>
+      <c r="M33" s="97"/>
+      <c r="N33" s="97"/>
+      <c r="O33" s="97"/>
     </row>
     <row r="34" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="72"/>
-      <c r="C34" s="63"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="64"/>
       <c r="D34" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="81"/>
       <c r="G34" s="11" t="s">
         <v>46</v>
       </c>
@@ -4758,17 +4831,17 @@
       </c>
     </row>
     <row r="35" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="72"/>
-      <c r="C35" s="63"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="64"/>
       <c r="D35" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="81"/>
       <c r="G35" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="103">
         <f>H4/H33</f>
         <v>1.2387152109474047E-7</v>
       </c>
@@ -4777,13 +4850,13 @@
       </c>
     </row>
     <row r="36" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="72"/>
-      <c r="C36" s="63"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="64"/>
       <c r="D36" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="81"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11">
         <f>SQRT(H35/(H39*10^-12))</f>
@@ -4792,13 +4865,13 @@
       <c r="I36" s="11"/>
     </row>
     <row r="37" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="72"/>
-      <c r="C37" s="63"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="64"/>
       <c r="D37" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="81"/>
       <c r="G37" s="11"/>
       <c r="H37" s="11">
         <f>SQRT(1/(H35*(H39*10^-12)))</f>
@@ -4807,13 +4880,13 @@
       <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:15" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="71"/>
-      <c r="C38" s="68"/>
+      <c r="B38" s="96"/>
+      <c r="C38" s="75"/>
       <c r="D38" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="75"/>
-      <c r="F38" s="76"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="98"/>
       <c r="G38" s="22"/>
       <c r="H38" s="22">
         <f>H24+(H4/H36)</f>
@@ -4822,11 +4895,11 @@
       <c r="I38" s="22"/>
     </row>
     <row r="39" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="69" t="s">
+      <c r="B39" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="66" t="s">
-        <v>66</v>
+      <c r="C39" s="63" t="s">
+        <v>65</v>
       </c>
       <c r="D39" s="32" t="s">
         <v>51</v>
@@ -4842,7 +4915,7 @@
         <v>53</v>
       </c>
       <c r="J39" s="62" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
       <c r="K39" s="62"/>
       <c r="L39" s="62"/>
@@ -4851,8 +4924,8 @@
       <c r="O39" s="62"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="72"/>
-      <c r="C40" s="63"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="64"/>
       <c r="G40" t="s">
         <v>57</v>
       </c>
@@ -4865,8 +4938,8 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="72"/>
-      <c r="C41" s="63"/>
+      <c r="B41" s="68"/>
+      <c r="C41" s="64"/>
       <c r="G41" t="s">
         <v>56</v>
       </c>
@@ -4879,8 +4952,8 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="72"/>
-      <c r="C42" s="63"/>
+      <c r="B42" s="68"/>
+      <c r="C42" s="64"/>
       <c r="G42" t="s">
         <v>59</v>
       </c>
@@ -4890,8 +4963,8 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="72"/>
-      <c r="C43" s="63"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="64"/>
       <c r="G43" t="s">
         <v>61</v>
       </c>
@@ -4904,10 +4977,10 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="72"/>
-      <c r="C44" s="63"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="64"/>
       <c r="G44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H44">
         <f>( (H34*H35)/H4)+(PI()/2)*SQRT(H35*(H39*10^-12))</f>
@@ -4918,15 +4991,15 @@
       </c>
     </row>
     <row r="45" spans="1:15" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="71"/>
-      <c r="C45" s="68"/>
+      <c r="B45" s="96"/>
+      <c r="C45" s="75"/>
       <c r="D45" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
       <c r="G45" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H45" s="22">
         <f>H38*SQRT(H44/H8)</f>
@@ -4937,44 +5010,44 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="69" t="s">
+      <c r="B46" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" t="s">
+        <v>88</v>
+      </c>
+      <c r="G46" s="59" t="s">
         <v>87</v>
-      </c>
-      <c r="C46" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="D46" t="s">
-        <v>89</v>
-      </c>
-      <c r="G46" s="59" t="s">
-        <v>88</v>
       </c>
       <c r="H46">
         <f>(H4*0.1)/((2*PI()*H47*H27*5.2))</f>
         <v>0.96720315252998001</v>
       </c>
-      <c r="J46" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="K46" s="65"/>
-      <c r="L46" s="65"/>
-      <c r="M46" s="65"/>
-      <c r="N46" s="65"/>
+      <c r="J46" s="79" t="s">
+        <v>90</v>
+      </c>
+      <c r="K46" s="79"/>
+      <c r="L46" s="79"/>
+      <c r="M46" s="79"/>
+      <c r="N46" s="79"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="70"/>
-      <c r="C47" s="67"/>
+      <c r="B47" s="72"/>
+      <c r="C47" s="74"/>
       <c r="D47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G47" s="59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H47">
         <v>10000</v>
       </c>
       <c r="I47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J47" s="46"/>
       <c r="K47" s="46"/>
@@ -4984,21 +5057,21 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="72"/>
+      <c r="C48" s="74"/>
+      <c r="D48" t="s">
+        <v>100</v>
+      </c>
+      <c r="G48" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="B48" s="70"/>
-      <c r="C48" s="67"/>
-      <c r="D48" t="s">
+      <c r="H48">
+        <v>250000</v>
+      </c>
+      <c r="I48" t="s">
         <v>101</v>
-      </c>
-      <c r="G48" s="59" t="s">
-        <v>97</v>
-      </c>
-      <c r="H48">
-        <v>125000</v>
-      </c>
-      <c r="I48" t="s">
-        <v>102</v>
       </c>
       <c r="J48" s="46"/>
       <c r="K48" s="46"/>
@@ -5007,79 +5080,79 @@
       <c r="N48" s="46"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="70"/>
-      <c r="C49" s="67"/>
+      <c r="B49" s="72"/>
+      <c r="C49" s="74"/>
       <c r="D49" s="19"/>
       <c r="E49" s="19"/>
       <c r="F49" s="19"/>
       <c r="G49" s="59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H49" s="19">
         <v>3300</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="70"/>
-      <c r="C50" s="67"/>
+      <c r="B50" s="72"/>
+      <c r="C50" s="74"/>
       <c r="G50" s="59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H50">
         <f>H49/H46</f>
         <v>3411.8995490946886</v>
       </c>
       <c r="I50" s="59" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="70"/>
-      <c r="C51" s="67"/>
+      <c r="B51" s="72"/>
+      <c r="C51" s="74"/>
       <c r="G51" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="H51">
+        <v>93</v>
+      </c>
+      <c r="H51" s="101">
         <f>1/(2*PI()*H47*H50)</f>
         <v>4.6647018999760829E-9</v>
       </c>
       <c r="I51" s="59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="71"/>
-      <c r="C52" s="68"/>
+      <c r="B52" s="96"/>
+      <c r="C52" s="75"/>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
       <c r="G52" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="H52" s="22">
+        <v>94</v>
+      </c>
+      <c r="H52" s="102">
         <f>1/(2*PI()*H50*H48)</f>
-        <v>3.7317615199808668E-10</v>
+        <v>1.8658807599904334E-10</v>
       </c>
       <c r="I52" s="60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>98</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="B53" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="D53" s="95" t="s">
+        <v>104</v>
+      </c>
+      <c r="E53" s="95"/>
+      <c r="G53" s="59" t="s">
         <v>103</v>
-      </c>
-      <c r="D53" s="61" t="s">
-        <v>105</v>
-      </c>
-      <c r="E53" s="61"/>
-      <c r="G53" s="59" t="s">
-        <v>104</v>
       </c>
       <c r="H53">
         <f>(H3)/(2*PI()*120*H28*H4)</f>
@@ -5090,8 +5163,10 @@
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="68"/>
+      <c r="C54" s="64"/>
       <c r="G54" s="59" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H54">
         <f>H53*2</f>
@@ -5102,91 +5177,159 @@
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="68"/>
+      <c r="C55" s="64"/>
       <c r="G55" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="H55">
+        <f>0.075</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I55" s="59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="68"/>
+      <c r="C56" s="64"/>
+      <c r="G56" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="H56">
+        <f>H55/H54</f>
+        <v>1.1489253133128385E-2</v>
+      </c>
+      <c r="I56" s="59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="68"/>
+      <c r="C57" s="64"/>
+      <c r="G57" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="H57">
+        <v>1360000</v>
+      </c>
+      <c r="I57" s="59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="68"/>
+      <c r="C58" s="64"/>
+      <c r="G58" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="H55">
-        <v>1360000</v>
-      </c>
-      <c r="I55" s="59" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G56" s="59" t="s">
+      <c r="H58">
+        <v>11239</v>
+      </c>
+      <c r="I58" s="59" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="68"/>
+      <c r="C59" s="64"/>
+      <c r="G59" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="H56">
-        <v>11239</v>
-      </c>
-      <c r="I56" s="59" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G57" s="59" t="s">
+      <c r="H59" s="99">
+        <f>1/(2*PI()*120*H56*H57)</f>
+        <v>8.4880548873167096E-8</v>
+      </c>
+      <c r="I59" s="59" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="68"/>
+      <c r="C60" s="64"/>
+      <c r="G60" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="H60">
+        <f xml:space="preserve"> H3/(2*PI()*H4*5*H28)</f>
+        <v>78.334073553042259</v>
+      </c>
+      <c r="I60" s="59"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="68"/>
+      <c r="C61" s="64"/>
+      <c r="G61" s="59" t="s">
+        <v>120</v>
+      </c>
+      <c r="H61">
+        <f>1/(2*PI()*H57*H59)</f>
+        <v>1.3787103759754062</v>
+      </c>
+      <c r="I61" s="59"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="68"/>
+      <c r="C62" s="64"/>
+      <c r="G62" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="H62">
+        <f>SQRT(H60*H61)</f>
+        <v>10.392304845413264</v>
+      </c>
+      <c r="I62" s="59"/>
+    </row>
+    <row r="63" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="96"/>
+      <c r="C63" s="75"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="H57">
-        <f>1/(2*PI()*120*0.009*H55)</f>
-        <v>1.0835712356474359E-7</v>
-      </c>
-      <c r="I57" s="59" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G58" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="H58" t="s">
-        <v>111</v>
+      <c r="H63" s="22">
+        <f>1/(2*PI()*H62*H59)</f>
+        <v>180426.39618622433</v>
+      </c>
+      <c r="I63" s="22"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>4.8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>121</v>
+      </c>
+      <c r="H64">
+        <f>7.5/H4</f>
+        <v>2.1428571428571429E-2</v>
+      </c>
+      <c r="I64">
+        <f>1/H64</f>
+        <v>46.666666666666664</v>
+      </c>
+    </row>
+    <row r="65" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>122</v>
+      </c>
+      <c r="H65">
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>123</v>
+      </c>
+      <c r="H66">
+        <f>(H64)*H65*(1+(H64))</f>
+        <v>43775.510204081627</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="56">
-    <mergeCell ref="J10:O12"/>
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="J27:O27"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="J25:O25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E7:F9"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="J19:O19"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C29:C31"/>
+  <mergeCells count="58">
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="J20:O20"/>
     <mergeCell ref="J46:N46"/>
@@ -5201,6 +5344,50 @@
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="C33:C38"/>
     <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C53:C63"/>
+    <mergeCell ref="B53:B63"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="J25:O25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E7:F9"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="J10:O12"/>
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="J27:O27"/>
+    <mergeCell ref="J24:O24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J30" r:id="rId1" display="https://www.digikey.com/product-detail/en/cree-wolfspeed/C3D06065I/C3D06065I-ND/5067191"/>
@@ -5212,4 +5399,162 @@
   <pageSetup scale="76" orientation="landscape" r:id="rId5"/>
   <drawing r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:R17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="79" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2">
+        <f>'Power Factor Correction'!H27</f>
+        <v>1.1075596590909088E-4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N2" s="104" t="s">
+        <v>133</v>
+      </c>
+      <c r="O2" t="s">
+        <v>127</v>
+      </c>
+      <c r="P2" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>129</v>
+      </c>
+      <c r="R2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3">
+        <f>'Power Factor Correction'!H24</f>
+        <v>7.7059314853766185</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>131</v>
+      </c>
+      <c r="M3">
+        <v>76</v>
+      </c>
+      <c r="N3" s="104">
+        <v>97</v>
+      </c>
+      <c r="O3">
+        <v>8.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>136</v>
+      </c>
+      <c r="M4">
+        <v>360</v>
+      </c>
+      <c r="N4" s="104">
+        <v>360</v>
+      </c>
+      <c r="O4">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>134</v>
+      </c>
+      <c r="M5">
+        <v>124</v>
+      </c>
+      <c r="N5" s="104">
+        <v>153</v>
+      </c>
+      <c r="O5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>135</v>
+      </c>
+      <c r="M6">
+        <f>SQRT(D2/(M5*10^-9))</f>
+        <v>29.886339244885953</v>
+      </c>
+      <c r="N6" s="104">
+        <f>SQRT($D$2/(N5*10^-9))</f>
+        <v>26.905300630548652</v>
+      </c>
+      <c r="O6" s="104">
+        <f>SQRT($D$2/(O5*10^-9))</f>
+        <v>33.280018916624861</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>137</v>
+      </c>
+      <c r="M7">
+        <f>($D$2*$D$3)/(ROUNDUP(M6,1)*M3*10^-6)</f>
+        <v>0.37558435349945551</v>
+      </c>
+      <c r="N7" s="104">
+        <f>($D$2*$D$3)/(ROUNDUP(N6,1)*N3*10^-6)</f>
+        <v>0.32587929930972231</v>
+      </c>
+      <c r="O7" s="104">
+        <f>($D$2*$D$3)/(ROUNDUP(O6,1)*O3*10^-6)</f>
+        <v>2.9058918949294958</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f>11.1*2*PI()*27</f>
+        <v>1883.0706365617218</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f>F16/1000</f>
+        <v>1.8830706365617218</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
competed rev 1 pcb design
</commit_message>
<xml_diff>
--- a/Power Factor Correction/Design Files/UC2855A Calculations (Autosaved).xlsx
+++ b/Power Factor Correction/Design Files/UC2855A Calculations (Autosaved).xlsx
@@ -465,8 +465,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
-    <numFmt numFmtId="179" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="180" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000000000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -831,48 +831,114 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -882,72 +948,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4116,7 +4116,7 @@
   <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4161,14 +4161,14 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="79" t="s">
+      <c r="J3" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
@@ -4192,15 +4192,15 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="68">
+      <c r="B7" s="78">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="78" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
       <c r="G7" t="s">
         <v>1</v>
       </c>
@@ -4209,11 +4209,11 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
       <c r="G8" t="s">
         <v>58</v>
       </c>
@@ -4223,11 +4223,11 @@
       </c>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
       <c r="G9" s="16" t="s">
         <v>2</v>
       </c>
@@ -4236,18 +4236,18 @@
         <v>1.7857142857142858E-10</v>
       </c>
       <c r="I9" s="16"/>
-      <c r="J9" s="79" t="s">
+      <c r="J9" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="K9" s="79"/>
-      <c r="L9" s="79"/>
-      <c r="M9" s="79"/>
-      <c r="N9" s="79"/>
-      <c r="O9" s="79"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="70"/>
+      <c r="N9" s="70"/>
+      <c r="O9" s="70"/>
     </row>
     <row r="10" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="47"/>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="99" t="s">
         <v>66</v>
       </c>
       <c r="D10" s="47" t="s">
@@ -4262,20 +4262,20 @@
       <c r="I10" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="62" t="s">
+      <c r="J10" s="69" t="s">
         <v>112</v>
       </c>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="69"/>
+      <c r="O10" s="69"/>
     </row>
     <row r="11" spans="2:15" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="73">
+      <c r="B11" s="99">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C11" s="64"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="14" t="s">
         <v>69</v>
       </c>
@@ -4288,16 +4288,16 @@
       <c r="I11" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="62"/>
-      <c r="K11" s="62"/>
-      <c r="L11" s="62"/>
-      <c r="M11" s="62"/>
-      <c r="N11" s="62"/>
-      <c r="O11" s="62"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="69"/>
+      <c r="O11" s="69"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
       <c r="D12" s="21" t="s">
         <v>111</v>
       </c>
@@ -4311,26 +4311,26 @@
       <c r="I12" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="62"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="62"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="62"/>
-      <c r="O12" s="62"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="69"/>
+      <c r="O12" s="69"/>
     </row>
     <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="37">
         <v>3</v>
       </c>
-      <c r="C13" s="85" t="s">
+      <c r="C13" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="85"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="96"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="96"/>
+      <c r="I13" s="96"/>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
@@ -4359,10 +4359,10 @@
       <c r="O14" s="17"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="71" t="s">
         <v>76</v>
       </c>
       <c r="D15" s="39"/>
@@ -4383,8 +4383,8 @@
       <c r="O15" s="38"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
       <c r="D16" s="43" t="s">
         <v>79</v>
       </c>
@@ -4431,16 +4431,16 @@
       <c r="O17" s="38"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="63">
+      <c r="B18" s="71">
         <v>3.2</v>
       </c>
-      <c r="C18" s="63" t="s">
+      <c r="C18" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="66" t="s">
+      <c r="D18" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="E18" s="66"/>
+      <c r="E18" s="74"/>
       <c r="F18" s="48"/>
       <c r="G18" s="19"/>
       <c r="H18" s="34">
@@ -4457,9 +4457,9 @@
       <c r="O18" s="49"/>
     </row>
     <row r="19" spans="2:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="64"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="68" t="s">
+      <c r="B19" s="77"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="78" t="s">
         <v>80</v>
       </c>
       <c r="E19" s="13"/>
@@ -4474,19 +4474,19 @@
       <c r="I19" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="J19" s="62" t="s">
+      <c r="J19" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="K19" s="62"/>
-      <c r="L19" s="62"/>
-      <c r="M19" s="62"/>
-      <c r="N19" s="62"/>
-      <c r="O19" s="62"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="68"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="78"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="19"/>
@@ -4497,18 +4497,18 @@
       <c r="I20" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="62" t="s">
+      <c r="J20" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="62"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="69"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
       <c r="D21" s="39" t="s">
         <v>84</v>
       </c>
@@ -4531,8 +4531,8 @@
       <c r="O21" s="38"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
+      <c r="B22" s="100"/>
+      <c r="C22" s="100"/>
       <c r="D22" s="14" t="s">
         <v>83</v>
       </c>
@@ -4541,7 +4541,7 @@
       <c r="G22" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="H22" s="100">
+      <c r="H22" s="63">
         <f>(3*H27*H18)/(H21*H4*H19)</f>
         <v>3.325238512566868E-11</v>
       </c>
@@ -4553,28 +4553,28 @@
       <c r="B23" s="3">
         <v>4.2</v>
       </c>
-      <c r="C23" s="70" t="s">
+      <c r="C23" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="70"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="97"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="2:15" ht="53.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="71" t="s">
+      <c r="B24" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="73" t="s">
+      <c r="C24" s="99" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
+      <c r="E24" s="94"/>
+      <c r="F24" s="94"/>
       <c r="G24" s="4" t="s">
         <v>13</v>
       </c>
@@ -4585,23 +4585,23 @@
       <c r="I24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J24" s="78" t="s">
+      <c r="J24" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="78"/>
-      <c r="L24" s="78"/>
-      <c r="M24" s="78"/>
-      <c r="N24" s="78"/>
-      <c r="O24" s="78"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="104"/>
+      <c r="M24" s="104"/>
+      <c r="N24" s="104"/>
+      <c r="O24" s="104"/>
     </row>
     <row r="25" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="72"/>
-      <c r="C25" s="74"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="72"/>
       <c r="D25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
       <c r="G25" s="5" t="s">
         <v>16</v>
       </c>
@@ -4612,21 +4612,21 @@
       <c r="I25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="82" t="s">
+      <c r="J25" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="K25" s="82"/>
-      <c r="L25" s="82"/>
-      <c r="M25" s="82"/>
-      <c r="N25" s="82"/>
-      <c r="O25" s="82"/>
+      <c r="K25" s="95"/>
+      <c r="L25" s="95"/>
+      <c r="M25" s="95"/>
+      <c r="N25" s="95"/>
+      <c r="O25" s="95"/>
     </row>
     <row r="26" spans="2:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="81"/>
-      <c r="F26" s="81"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
       <c r="G26" s="10" t="s">
         <v>21</v>
       </c>
@@ -4648,8 +4648,8 @@
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
+      <c r="E27" s="102"/>
+      <c r="F27" s="102"/>
       <c r="G27" s="21" t="s">
         <v>23</v>
       </c>
@@ -4660,12 +4660,12 @@
       <c r="I27" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="77"/>
-      <c r="K27" s="77"/>
-      <c r="L27" s="77"/>
-      <c r="M27" s="77"/>
-      <c r="N27" s="77"/>
-      <c r="O27" s="77"/>
+      <c r="J27" s="103"/>
+      <c r="K27" s="103"/>
+      <c r="L27" s="103"/>
+      <c r="M27" s="103"/>
+      <c r="N27" s="103"/>
+      <c r="O27" s="103"/>
     </row>
     <row r="28" spans="2:15" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
@@ -4677,8 +4677,8 @@
       <c r="D28" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
       <c r="G28" s="23" t="s">
         <v>28</v>
       </c>
@@ -4687,75 +4687,75 @@
         <v>5.1083900226757363E-4</v>
       </c>
       <c r="I28" s="25"/>
-      <c r="J28" s="67" t="s">
+      <c r="J28" s="101" t="s">
         <v>115</v>
       </c>
-      <c r="K28" s="67"/>
-      <c r="L28" s="67"/>
-      <c r="M28" s="67"/>
-      <c r="N28" s="67"/>
+      <c r="K28" s="101"/>
+      <c r="L28" s="101"/>
+      <c r="M28" s="101"/>
+      <c r="N28" s="101"/>
     </row>
     <row r="29" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="64" t="s">
+      <c r="C29" s="77" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="87" t="s">
+      <c r="E29" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
+      <c r="F29" s="91"/>
+      <c r="G29" s="91"/>
+      <c r="H29" s="91"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="88" t="s">
+      <c r="J29" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="K29" s="88"/>
+      <c r="K29" s="92"/>
       <c r="L29" t="s">
         <v>33</v>
       </c>
-      <c r="M29" s="88" t="s">
+      <c r="M29" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="N29" s="88"/>
+      <c r="N29" s="92"/>
     </row>
     <row r="30" spans="2:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="68"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="92" t="s">
+      <c r="B30" s="78"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="89" t="s">
+      <c r="E30" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="89"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="89"/>
-      <c r="J30" s="88" t="s">
+      <c r="F30" s="93"/>
+      <c r="G30" s="93"/>
+      <c r="H30" s="93"/>
+      <c r="J30" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="K30" s="88"/>
+      <c r="K30" s="92"/>
       <c r="L30" t="s">
         <v>33</v>
       </c>
-      <c r="M30" s="88" t="s">
+      <c r="M30" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="N30" s="88"/>
+      <c r="N30" s="92"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="69"/>
-      <c r="C31" s="94"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="84" t="s">
+      <c r="B31" s="88"/>
+      <c r="C31" s="87"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="84"/>
+      <c r="F31" s="89"/>
       <c r="G31" s="20" t="s">
         <v>38</v>
       </c>
@@ -4770,28 +4770,28 @@
       <c r="B32" s="27">
         <v>4.3</v>
       </c>
-      <c r="C32" s="90" t="s">
+      <c r="C32" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="90"/>
-      <c r="G32" s="90"/>
-      <c r="H32" s="90"/>
-      <c r="I32" s="90"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="83"/>
     </row>
     <row r="33" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="66" t="s">
+      <c r="B33" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="63" t="s">
+      <c r="C33" s="71" t="s">
         <v>42</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="84"/>
       <c r="G33" s="28" t="s">
         <v>47</v>
       </c>
@@ -4802,23 +4802,23 @@
       <c r="I33" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="J33" s="97" t="s">
+      <c r="J33" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="K33" s="97"/>
-      <c r="L33" s="97"/>
-      <c r="M33" s="97"/>
-      <c r="N33" s="97"/>
-      <c r="O33" s="97"/>
+      <c r="K33" s="79"/>
+      <c r="L33" s="79"/>
+      <c r="M33" s="79"/>
+      <c r="N33" s="79"/>
+      <c r="O33" s="79"/>
     </row>
     <row r="34" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="68"/>
-      <c r="C34" s="64"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="77"/>
       <c r="D34" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
       <c r="G34" s="11" t="s">
         <v>46</v>
       </c>
@@ -4831,17 +4831,17 @@
       </c>
     </row>
     <row r="35" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="68"/>
-      <c r="C35" s="64"/>
+      <c r="B35" s="78"/>
+      <c r="C35" s="77"/>
       <c r="D35" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
       <c r="G35" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="H35" s="103">
+      <c r="H35" s="66">
         <f>H4/H33</f>
         <v>1.2387152109474047E-7</v>
       </c>
@@ -4850,13 +4850,13 @@
       </c>
     </row>
     <row r="36" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="68"/>
-      <c r="C36" s="64"/>
+      <c r="B36" s="78"/>
+      <c r="C36" s="77"/>
       <c r="D36" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11">
         <f>SQRT(H35/(H39*10^-12))</f>
@@ -4865,13 +4865,13 @@
       <c r="I36" s="11"/>
     </row>
     <row r="37" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="68"/>
-      <c r="C37" s="64"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="77"/>
       <c r="D37" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
       <c r="G37" s="11"/>
       <c r="H37" s="11">
         <f>SQRT(1/(H35*(H39*10^-12)))</f>
@@ -4880,13 +4880,13 @@
       <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:15" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="96"/>
-      <c r="C38" s="75"/>
+      <c r="B38" s="76"/>
+      <c r="C38" s="73"/>
       <c r="D38" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="83"/>
-      <c r="F38" s="98"/>
+      <c r="E38" s="81"/>
+      <c r="F38" s="82"/>
       <c r="G38" s="22"/>
       <c r="H38" s="22">
         <f>H24+(H4/H36)</f>
@@ -4895,10 +4895,10 @@
       <c r="I38" s="22"/>
     </row>
     <row r="39" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="66" t="s">
+      <c r="B39" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="63" t="s">
+      <c r="C39" s="71" t="s">
         <v>65</v>
       </c>
       <c r="D39" s="32" t="s">
@@ -4914,18 +4914,18 @@
       <c r="I39" t="s">
         <v>53</v>
       </c>
-      <c r="J39" s="62" t="s">
+      <c r="J39" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="K39" s="62"/>
-      <c r="L39" s="62"/>
-      <c r="M39" s="62"/>
-      <c r="N39" s="62"/>
-      <c r="O39" s="62"/>
+      <c r="K39" s="69"/>
+      <c r="L39" s="69"/>
+      <c r="M39" s="69"/>
+      <c r="N39" s="69"/>
+      <c r="O39" s="69"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="68"/>
-      <c r="C40" s="64"/>
+      <c r="B40" s="78"/>
+      <c r="C40" s="77"/>
       <c r="G40" t="s">
         <v>57</v>
       </c>
@@ -4938,8 +4938,8 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="68"/>
-      <c r="C41" s="64"/>
+      <c r="B41" s="78"/>
+      <c r="C41" s="77"/>
       <c r="G41" t="s">
         <v>56</v>
       </c>
@@ -4952,8 +4952,8 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="68"/>
-      <c r="C42" s="64"/>
+      <c r="B42" s="78"/>
+      <c r="C42" s="77"/>
       <c r="G42" t="s">
         <v>59</v>
       </c>
@@ -4963,8 +4963,8 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="68"/>
-      <c r="C43" s="64"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="77"/>
       <c r="G43" t="s">
         <v>61</v>
       </c>
@@ -4977,8 +4977,8 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="68"/>
-      <c r="C44" s="64"/>
+      <c r="B44" s="78"/>
+      <c r="C44" s="77"/>
       <c r="G44" t="s">
         <v>62</v>
       </c>
@@ -4991,8 +4991,8 @@
       </c>
     </row>
     <row r="45" spans="1:15" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="96"/>
-      <c r="C45" s="75"/>
+      <c r="B45" s="76"/>
+      <c r="C45" s="73"/>
       <c r="D45" s="42" t="s">
         <v>64</v>
       </c>
@@ -5010,10 +5010,10 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="66" t="s">
+      <c r="B46" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="63" t="s">
+      <c r="C46" s="71" t="s">
         <v>98</v>
       </c>
       <c r="D46" t="s">
@@ -5026,17 +5026,17 @@
         <f>(H4*0.1)/((2*PI()*H47*H27*5.2))</f>
         <v>0.96720315252998001</v>
       </c>
-      <c r="J46" s="79" t="s">
+      <c r="J46" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="K46" s="79"/>
-      <c r="L46" s="79"/>
-      <c r="M46" s="79"/>
-      <c r="N46" s="79"/>
+      <c r="K46" s="70"/>
+      <c r="L46" s="70"/>
+      <c r="M46" s="70"/>
+      <c r="N46" s="70"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="72"/>
-      <c r="C47" s="74"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="72"/>
       <c r="D47" t="s">
         <v>99</v>
       </c>
@@ -5059,8 +5059,8 @@
       <c r="A48" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="72"/>
-      <c r="C48" s="74"/>
+      <c r="B48" s="75"/>
+      <c r="C48" s="72"/>
       <c r="D48" t="s">
         <v>100</v>
       </c>
@@ -5080,8 +5080,8 @@
       <c r="N48" s="46"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="72"/>
-      <c r="C49" s="74"/>
+      <c r="B49" s="75"/>
+      <c r="C49" s="72"/>
       <c r="D49" s="19"/>
       <c r="E49" s="19"/>
       <c r="F49" s="19"/>
@@ -5096,8 +5096,8 @@
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="72"/>
-      <c r="C50" s="74"/>
+      <c r="B50" s="75"/>
+      <c r="C50" s="72"/>
       <c r="G50" s="59" t="s">
         <v>91</v>
       </c>
@@ -5110,12 +5110,12 @@
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="72"/>
-      <c r="C51" s="74"/>
+      <c r="B51" s="75"/>
+      <c r="C51" s="72"/>
       <c r="G51" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="H51" s="101">
+      <c r="H51" s="64">
         <f>1/(2*PI()*H47*H50)</f>
         <v>4.6647018999760829E-9</v>
       </c>
@@ -5124,15 +5124,15 @@
       </c>
     </row>
     <row r="52" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="96"/>
-      <c r="C52" s="75"/>
+      <c r="B52" s="76"/>
+      <c r="C52" s="73"/>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
       <c r="G52" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="H52" s="102">
+      <c r="H52" s="65">
         <f>1/(2*PI()*H50*H48)</f>
         <v>1.8658807599904334E-10</v>
       </c>
@@ -5141,16 +5141,16 @@
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="66" t="s">
+      <c r="B53" s="74" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="63" t="s">
+      <c r="C53" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="D53" s="95" t="s">
+      <c r="D53" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="95"/>
+      <c r="E53" s="68"/>
       <c r="G53" s="59" t="s">
         <v>103</v>
       </c>
@@ -5163,8 +5163,8 @@
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="68"/>
-      <c r="C54" s="64"/>
+      <c r="B54" s="78"/>
+      <c r="C54" s="77"/>
       <c r="G54" s="59" t="s">
         <v>105</v>
       </c>
@@ -5177,8 +5177,8 @@
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="68"/>
-      <c r="C55" s="64"/>
+      <c r="B55" s="78"/>
+      <c r="C55" s="77"/>
       <c r="G55" s="59" t="s">
         <v>116</v>
       </c>
@@ -5191,8 +5191,8 @@
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="68"/>
-      <c r="C56" s="64"/>
+      <c r="B56" s="78"/>
+      <c r="C56" s="77"/>
       <c r="G56" s="59" t="s">
         <v>117</v>
       </c>
@@ -5205,8 +5205,8 @@
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="68"/>
-      <c r="C57" s="64"/>
+      <c r="B57" s="78"/>
+      <c r="C57" s="77"/>
       <c r="G57" s="59" t="s">
         <v>106</v>
       </c>
@@ -5218,8 +5218,8 @@
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="68"/>
-      <c r="C58" s="64"/>
+      <c r="B58" s="78"/>
+      <c r="C58" s="77"/>
       <c r="G58" s="59" t="s">
         <v>107</v>
       </c>
@@ -5231,12 +5231,12 @@
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="68"/>
-      <c r="C59" s="64"/>
+      <c r="B59" s="78"/>
+      <c r="C59" s="77"/>
       <c r="G59" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="H59" s="99">
+      <c r="H59" s="62">
         <f>1/(2*PI()*120*H56*H57)</f>
         <v>8.4880548873167096E-8</v>
       </c>
@@ -5245,8 +5245,8 @@
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="68"/>
-      <c r="C60" s="64"/>
+      <c r="B60" s="78"/>
+      <c r="C60" s="77"/>
       <c r="G60" s="59" t="s">
         <v>118</v>
       </c>
@@ -5257,8 +5257,8 @@
       <c r="I60" s="59"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="68"/>
-      <c r="C61" s="64"/>
+      <c r="B61" s="78"/>
+      <c r="C61" s="77"/>
       <c r="G61" s="59" t="s">
         <v>120</v>
       </c>
@@ -5269,8 +5269,8 @@
       <c r="I61" s="59"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="68"/>
-      <c r="C62" s="64"/>
+      <c r="B62" s="78"/>
+      <c r="C62" s="77"/>
       <c r="G62" s="59" t="s">
         <v>119</v>
       </c>
@@ -5281,8 +5281,8 @@
       <c r="I62" s="59"/>
     </row>
     <row r="63" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="96"/>
-      <c r="C63" s="75"/>
+      <c r="B63" s="76"/>
+      <c r="C63" s="73"/>
       <c r="D63" s="22"/>
       <c r="E63" s="22"/>
       <c r="F63" s="22"/>
@@ -5330,6 +5330,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="J27:O27"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="J25:O25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E7:F9"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J10:O12"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C29:C31"/>
     <mergeCell ref="D53:E53"/>
     <mergeCell ref="J20:O20"/>
     <mergeCell ref="J46:N46"/>
@@ -5346,48 +5388,6 @@
     <mergeCell ref="B33:B38"/>
     <mergeCell ref="C53:C63"/>
     <mergeCell ref="B53:B63"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="J25:O25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E7:F9"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="J19:O19"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="J10:O12"/>
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="J27:O27"/>
-    <mergeCell ref="J24:O24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J30" r:id="rId1" display="https://www.digikey.com/product-detail/en/cree-wolfspeed/C3D06065I/C3D06065I-ND/5067191"/>
@@ -5418,11 +5418,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="70" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
       <c r="D2">
         <f>'Power Factor Correction'!H27</f>
         <v>1.1075596590909088E-4</v>
@@ -5433,7 +5433,7 @@
       <c r="M2" t="s">
         <v>132</v>
       </c>
-      <c r="N2" s="104" t="s">
+      <c r="N2" s="67" t="s">
         <v>133</v>
       </c>
       <c r="O2" t="s">
@@ -5450,11 +5450,11 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="70" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
       <c r="D3">
         <f>'Power Factor Correction'!H24</f>
         <v>7.7059314853766185</v>
@@ -5468,7 +5468,7 @@
       <c r="M3">
         <v>76</v>
       </c>
-      <c r="N3" s="104">
+      <c r="N3" s="67">
         <v>97</v>
       </c>
       <c r="O3">
@@ -5482,7 +5482,7 @@
       <c r="M4">
         <v>360</v>
       </c>
-      <c r="N4" s="104">
+      <c r="N4" s="67">
         <v>360</v>
       </c>
       <c r="O4">
@@ -5496,7 +5496,7 @@
       <c r="M5">
         <v>124</v>
       </c>
-      <c r="N5" s="104">
+      <c r="N5" s="67">
         <v>153</v>
       </c>
       <c r="O5">
@@ -5511,11 +5511,11 @@
         <f>SQRT(D2/(M5*10^-9))</f>
         <v>29.886339244885953</v>
       </c>
-      <c r="N6" s="104">
+      <c r="N6" s="67">
         <f>SQRT($D$2/(N5*10^-9))</f>
         <v>26.905300630548652</v>
       </c>
-      <c r="O6" s="104">
+      <c r="O6" s="67">
         <f>SQRT($D$2/(O5*10^-9))</f>
         <v>33.280018916624861</v>
       </c>
@@ -5528,11 +5528,11 @@
         <f>($D$2*$D$3)/(ROUNDUP(M6,1)*M3*10^-6)</f>
         <v>0.37558435349945551</v>
       </c>
-      <c r="N7" s="104">
+      <c r="N7" s="67">
         <f>($D$2*$D$3)/(ROUNDUP(N6,1)*N3*10^-6)</f>
         <v>0.32587929930972231</v>
       </c>
-      <c r="O7" s="104">
+      <c r="O7" s="67">
         <f>($D$2*$D$3)/(ROUNDUP(O6,1)*O3*10^-6)</f>
         <v>2.9058918949294958</v>
       </c>

</xml_diff>

<commit_message>
working on REV2 of PFC PCB
</commit_message>
<xml_diff>
--- a/Power Factor Correction/Design Files/UC2855A Calculations (Autosaved).xlsx
+++ b/Power Factor Correction/Design Files/UC2855A Calculations (Autosaved).xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="142">
   <si>
     <t>Oscillator</t>
   </si>
@@ -428,9 +428,6 @@
     <t>ETD39</t>
   </si>
   <si>
-    <t>ETD44</t>
-  </si>
-  <si>
     <t>ETD49</t>
   </si>
   <si>
@@ -456,6 +453,21 @@
   </si>
   <si>
     <t>B  Calculated</t>
+  </si>
+  <si>
+    <t>Current Transformer</t>
+  </si>
+  <si>
+    <t>Saturation Current</t>
+  </si>
+  <si>
+    <t>ETD44 1.00mm Gap</t>
+  </si>
+  <si>
+    <t>ETD44 1.5mm Gap</t>
+  </si>
+  <si>
+    <t>GEA</t>
   </si>
 </sst>
 </file>
@@ -468,7 +480,7 @@
     <numFmt numFmtId="166" formatCode="0.00000000000000"/>
     <numFmt numFmtId="167" formatCode="0.000000000000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,8 +522,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,6 +541,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -676,11 +700,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -833,123 +858,134 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -4113,10 +4149,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O66"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4161,14 +4197,14 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="70" t="s">
+      <c r="J3" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
@@ -4192,15 +4228,15 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="78">
+      <c r="B7" s="72">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C7" s="78" t="s">
+      <c r="C7" s="72" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
       <c r="G7" t="s">
         <v>1</v>
       </c>
@@ -4209,11 +4245,11 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
       <c r="G8" t="s">
         <v>58</v>
       </c>
@@ -4223,8 +4259,8 @@
       </c>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
       <c r="D9" s="15"/>
       <c r="E9" s="89"/>
       <c r="F9" s="89"/>
@@ -4236,18 +4272,18 @@
         <v>1.7857142857142858E-10</v>
       </c>
       <c r="I9" s="16"/>
-      <c r="J9" s="70" t="s">
+      <c r="J9" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="K9" s="70"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="70"/>
-      <c r="N9" s="70"/>
-      <c r="O9" s="70"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="84"/>
+      <c r="N9" s="84"/>
+      <c r="O9" s="84"/>
     </row>
     <row r="10" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="47"/>
-      <c r="C10" s="99" t="s">
+      <c r="C10" s="77" t="s">
         <v>66</v>
       </c>
       <c r="D10" s="47" t="s">
@@ -4262,20 +4298,20 @@
       <c r="I10" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="69" t="s">
+      <c r="J10" s="91" t="s">
         <v>112</v>
       </c>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="69"/>
+      <c r="K10" s="91"/>
+      <c r="L10" s="91"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="91"/>
+      <c r="O10" s="91"/>
     </row>
     <row r="11" spans="2:15" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="99">
+      <c r="B11" s="77">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C11" s="77"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="14" t="s">
         <v>69</v>
       </c>
@@ -4288,16 +4324,16 @@
       <c r="I11" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="69"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
-      <c r="O11" s="69"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="91"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91"/>
+      <c r="O11" s="91"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="21" t="s">
         <v>111</v>
       </c>
@@ -4311,26 +4347,26 @@
       <c r="I12" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
+      <c r="J12" s="91"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="91"/>
+      <c r="M12" s="91"/>
+      <c r="N12" s="91"/>
+      <c r="O12" s="91"/>
     </row>
     <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="37">
         <v>3</v>
       </c>
-      <c r="C13" s="96" t="s">
+      <c r="C13" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="96"/>
-      <c r="G13" s="96"/>
-      <c r="H13" s="96"/>
-      <c r="I13" s="96"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
@@ -4359,10 +4395,10 @@
       <c r="O14" s="17"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="80" t="s">
         <v>76</v>
       </c>
       <c r="D15" s="39"/>
@@ -4383,8 +4419,8 @@
       <c r="O15" s="38"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="79"/>
       <c r="D16" s="43" t="s">
         <v>79</v>
       </c>
@@ -4431,16 +4467,16 @@
       <c r="O17" s="38"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="71">
+      <c r="B18" s="80">
         <v>3.2</v>
       </c>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="E18" s="74"/>
+      <c r="E18" s="83"/>
       <c r="F18" s="48"/>
       <c r="G18" s="19"/>
       <c r="H18" s="34">
@@ -4457,9 +4493,9 @@
       <c r="O18" s="49"/>
     </row>
     <row r="19" spans="2:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="77"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="78" t="s">
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="72" t="s">
         <v>80</v>
       </c>
       <c r="E19" s="13"/>
@@ -4468,25 +4504,25 @@
         <v>80</v>
       </c>
       <c r="H19" s="34">
-        <f>1/(H24/H18)</f>
+        <f>1/((H24)/H18)</f>
         <v>12.977016495639477</v>
       </c>
       <c r="I19" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="J19" s="69" t="s">
+      <c r="J19" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="K19" s="69"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
+      <c r="K19" s="91"/>
+      <c r="L19" s="91"/>
+      <c r="M19" s="91"/>
+      <c r="N19" s="91"/>
+      <c r="O19" s="91"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="77"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="78"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="72"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="19"/>
@@ -4497,18 +4533,18 @@
       <c r="I20" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="69" t="s">
+      <c r="J20" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
+      <c r="K20" s="91"/>
+      <c r="L20" s="91"/>
+      <c r="M20" s="91"/>
+      <c r="N20" s="91"/>
+      <c r="O20" s="91"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
       <c r="D21" s="39" t="s">
         <v>84</v>
       </c>
@@ -4531,8 +4567,8 @@
       <c r="O21" s="38"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="100"/>
-      <c r="C22" s="100"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="82"/>
       <c r="D22" s="14" t="s">
         <v>83</v>
       </c>
@@ -4553,28 +4589,28 @@
       <c r="B23" s="3">
         <v>4.2</v>
       </c>
-      <c r="C23" s="97" t="s">
+      <c r="C23" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="97"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
-      <c r="G23" s="97"/>
-      <c r="H23" s="97"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="2:15" ht="53.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="99" t="s">
+      <c r="C24" s="77" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="94"/>
-      <c r="F24" s="94"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="85"/>
       <c r="G24" s="4" t="s">
         <v>13</v>
       </c>
@@ -4585,23 +4621,23 @@
       <c r="I24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J24" s="104" t="s">
+      <c r="J24" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="104"/>
-      <c r="L24" s="104"/>
-      <c r="M24" s="104"/>
-      <c r="N24" s="104"/>
-      <c r="O24" s="104"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="71"/>
+      <c r="N24" s="71"/>
+      <c r="O24" s="71"/>
     </row>
     <row r="25" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="75"/>
-      <c r="C25" s="72"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="78"/>
       <c r="D25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
       <c r="G25" s="5" t="s">
         <v>16</v>
       </c>
@@ -4612,21 +4648,21 @@
       <c r="I25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="95" t="s">
+      <c r="J25" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="K25" s="95"/>
-      <c r="L25" s="95"/>
-      <c r="M25" s="95"/>
-      <c r="N25" s="95"/>
-      <c r="O25" s="95"/>
+      <c r="K25" s="87"/>
+      <c r="L25" s="87"/>
+      <c r="M25" s="87"/>
+      <c r="N25" s="87"/>
+      <c r="O25" s="87"/>
     </row>
     <row r="26" spans="2:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="80"/>
-      <c r="F26" s="80"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
       <c r="G26" s="10" t="s">
         <v>21</v>
       </c>
@@ -4648,8 +4684,8 @@
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
-      <c r="E27" s="102"/>
-      <c r="F27" s="102"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
       <c r="G27" s="21" t="s">
         <v>23</v>
       </c>
@@ -4660,12 +4696,12 @@
       <c r="I27" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="103"/>
-      <c r="K27" s="103"/>
-      <c r="L27" s="103"/>
-      <c r="M27" s="103"/>
-      <c r="N27" s="103"/>
-      <c r="O27" s="103"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="70"/>
+      <c r="L27" s="70"/>
+      <c r="M27" s="70"/>
+      <c r="N27" s="70"/>
+      <c r="O27" s="70"/>
     </row>
     <row r="28" spans="2:15" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
@@ -4677,8 +4713,8 @@
       <c r="D28" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="90"/>
-      <c r="F28" s="90"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="92"/>
       <c r="G28" s="23" t="s">
         <v>28</v>
       </c>
@@ -4687,71 +4723,71 @@
         <v>5.1083900226757363E-4</v>
       </c>
       <c r="I28" s="25"/>
-      <c r="J28" s="101" t="s">
+      <c r="J28" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="K28" s="101"/>
-      <c r="L28" s="101"/>
-      <c r="M28" s="101"/>
-      <c r="N28" s="101"/>
+      <c r="K28" s="96"/>
+      <c r="L28" s="96"/>
+      <c r="M28" s="96"/>
+      <c r="N28" s="96"/>
     </row>
     <row r="29" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="78" t="s">
+      <c r="B29" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="77" t="s">
+      <c r="C29" s="81" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="91" t="s">
+      <c r="E29" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="91"/>
-      <c r="G29" s="91"/>
-      <c r="H29" s="91"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="93"/>
+      <c r="H29" s="93"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="92" t="s">
+      <c r="J29" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="K29" s="92"/>
+      <c r="K29" s="94"/>
       <c r="L29" t="s">
         <v>33</v>
       </c>
-      <c r="M29" s="92" t="s">
+      <c r="M29" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="N29" s="92"/>
+      <c r="N29" s="94"/>
     </row>
     <row r="30" spans="2:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="78"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="85" t="s">
+      <c r="B30" s="72"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="93" t="s">
+      <c r="E30" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="93"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="93"/>
-      <c r="J30" s="92" t="s">
+      <c r="F30" s="95"/>
+      <c r="G30" s="95"/>
+      <c r="H30" s="95"/>
+      <c r="J30" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="K30" s="92"/>
+      <c r="K30" s="94"/>
       <c r="L30" t="s">
         <v>33</v>
       </c>
-      <c r="M30" s="92" t="s">
+      <c r="M30" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="N30" s="92"/>
+      <c r="N30" s="94"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="88"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="86"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="100"/>
       <c r="E31" s="89" t="s">
         <v>39</v>
       </c>
@@ -4770,28 +4806,28 @@
       <c r="B32" s="27">
         <v>4.3</v>
       </c>
-      <c r="C32" s="83" t="s">
+      <c r="C32" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="83"/>
-      <c r="E32" s="83"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="83"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="83"/>
-    </row>
-    <row r="33" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="74" t="s">
+      <c r="D32" s="97"/>
+      <c r="E32" s="97"/>
+      <c r="F32" s="97"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="97"/>
+    </row>
+    <row r="33" spans="2:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="71" t="s">
+      <c r="C33" s="80" t="s">
         <v>42</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="84"/>
-      <c r="F33" s="84"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="98"/>
       <c r="G33" s="28" t="s">
         <v>47</v>
       </c>
@@ -4802,23 +4838,23 @@
       <c r="I33" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="J33" s="79" t="s">
+      <c r="J33" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="K33" s="79"/>
-      <c r="L33" s="79"/>
-      <c r="M33" s="79"/>
-      <c r="N33" s="79"/>
-      <c r="O33" s="79"/>
-    </row>
-    <row r="34" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="78"/>
-      <c r="C34" s="77"/>
+      <c r="K33" s="104"/>
+      <c r="L33" s="104"/>
+      <c r="M33" s="104"/>
+      <c r="N33" s="104"/>
+      <c r="O33" s="104"/>
+    </row>
+    <row r="34" spans="2:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="72"/>
+      <c r="C34" s="81"/>
       <c r="D34" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="80"/>
-      <c r="F34" s="80"/>
+      <c r="E34" s="86"/>
+      <c r="F34" s="86"/>
       <c r="G34" s="11" t="s">
         <v>46</v>
       </c>
@@ -4830,18 +4866,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="78"/>
-      <c r="C35" s="77"/>
+    <row r="35" spans="2:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="72"/>
+      <c r="C35" s="81"/>
       <c r="D35" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="80"/>
-      <c r="F35" s="80"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="86"/>
       <c r="G35" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="H35" s="66">
+      <c r="H35" s="64">
         <f>H4/H33</f>
         <v>1.2387152109474047E-7</v>
       </c>
@@ -4849,14 +4885,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="78"/>
-      <c r="C36" s="77"/>
+    <row r="36" spans="2:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="72"/>
+      <c r="C36" s="81"/>
       <c r="D36" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="80"/>
-      <c r="F36" s="80"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="86"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11">
         <f>SQRT(H35/(H39*10^-12))</f>
@@ -4864,14 +4900,14 @@
       </c>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="1:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="78"/>
-      <c r="C37" s="77"/>
+    <row r="37" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="72"/>
+      <c r="C37" s="81"/>
       <c r="D37" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="80"/>
-      <c r="F37" s="80"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
       <c r="G37" s="11"/>
       <c r="H37" s="11">
         <f>SQRT(1/(H35*(H39*10^-12)))</f>
@@ -4879,14 +4915,14 @@
       </c>
       <c r="I37" s="11"/>
     </row>
-    <row r="38" spans="1:15" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="76"/>
-      <c r="C38" s="73"/>
+    <row r="38" spans="2:15" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="103"/>
+      <c r="C38" s="79"/>
       <c r="D38" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="81"/>
-      <c r="F38" s="82"/>
+      <c r="E38" s="88"/>
+      <c r="F38" s="105"/>
       <c r="G38" s="22"/>
       <c r="H38" s="22">
         <f>H24+(H4/H36)</f>
@@ -4894,11 +4930,11 @@
       </c>
       <c r="I38" s="22"/>
     </row>
-    <row r="39" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="74" t="s">
+    <row r="39" spans="2:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="71" t="s">
+      <c r="C39" s="80" t="s">
         <v>65</v>
       </c>
       <c r="D39" s="32" t="s">
@@ -4914,18 +4950,18 @@
       <c r="I39" t="s">
         <v>53</v>
       </c>
-      <c r="J39" s="69" t="s">
+      <c r="J39" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="K39" s="69"/>
-      <c r="L39" s="69"/>
-      <c r="M39" s="69"/>
-      <c r="N39" s="69"/>
-      <c r="O39" s="69"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="78"/>
-      <c r="C40" s="77"/>
+      <c r="K39" s="91"/>
+      <c r="L39" s="91"/>
+      <c r="M39" s="91"/>
+      <c r="N39" s="91"/>
+      <c r="O39" s="91"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="72"/>
+      <c r="C40" s="81"/>
       <c r="G40" t="s">
         <v>57</v>
       </c>
@@ -4937,9 +4973,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="78"/>
-      <c r="C41" s="77"/>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="72"/>
+      <c r="C41" s="81"/>
       <c r="G41" t="s">
         <v>56</v>
       </c>
@@ -4951,9 +4987,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="78"/>
-      <c r="C42" s="77"/>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="72"/>
+      <c r="C42" s="81"/>
       <c r="G42" t="s">
         <v>59</v>
       </c>
@@ -4962,9 +4998,9 @@
         <v>4.8917086585538961E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="78"/>
-      <c r="C43" s="77"/>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="72"/>
+      <c r="C43" s="81"/>
       <c r="G43" t="s">
         <v>61</v>
       </c>
@@ -4976,9 +5012,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="78"/>
-      <c r="C44" s="77"/>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B44" s="72"/>
+      <c r="C44" s="81"/>
       <c r="G44" t="s">
         <v>62</v>
       </c>
@@ -4990,9 +5026,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="76"/>
-      <c r="C45" s="73"/>
+    <row r="45" spans="2:15" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="103"/>
+      <c r="C45" s="79"/>
       <c r="D45" s="42" t="s">
         <v>64</v>
       </c>
@@ -5009,327 +5045,412 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="74" t="s">
+    <row r="46" spans="2:15" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="68">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C46" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" s="67"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+    </row>
+    <row r="47" spans="2:15" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="68"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="71" t="s">
+      <c r="C48" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D48" t="s">
         <v>88</v>
       </c>
-      <c r="G46" s="59" t="s">
+      <c r="G48" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="H46">
-        <f>(H4*0.1)/((2*PI()*H47*H27*5.2))</f>
-        <v>0.96720315252998001</v>
-      </c>
-      <c r="J46" s="70" t="s">
+      <c r="H48">
+        <f>(H4*((1/H18)*H19)/((2*PI()*H50*H27*5.2)))</f>
+        <v>1.2551411265016057</v>
+      </c>
+      <c r="J48" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="K46" s="70"/>
-      <c r="L46" s="70"/>
-      <c r="M46" s="70"/>
-      <c r="N46" s="70"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="75"/>
-      <c r="C47" s="72"/>
-      <c r="D47" t="s">
+      <c r="K48" s="84"/>
+      <c r="L48" s="84"/>
+      <c r="M48" s="84"/>
+      <c r="N48" s="84"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B49" s="72"/>
+      <c r="C49" s="81"/>
+      <c r="G49" s="59" t="s">
+        <v>141</v>
+      </c>
+      <c r="H49">
+        <f>1/H48</f>
+        <v>0.79672315637306201</v>
+      </c>
+      <c r="J49" s="66"/>
+      <c r="K49" s="66"/>
+      <c r="L49" s="66"/>
+      <c r="M49" s="66"/>
+      <c r="N49" s="66"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B50" s="76"/>
+      <c r="C50" s="78"/>
+      <c r="D50" t="s">
         <v>99</v>
       </c>
-      <c r="G47" s="59" t="s">
+      <c r="G50" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="H47">
+      <c r="H50">
         <v>10000</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I50" t="s">
         <v>101</v>
       </c>
-      <c r="J47" s="46"/>
-      <c r="K47" s="46"/>
-      <c r="L47" s="46"/>
-      <c r="M47" s="46"/>
-      <c r="N47" s="46"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="J50" s="46"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="46"/>
+      <c r="M50" s="46"/>
+      <c r="N50" s="46"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="75"/>
-      <c r="C48" s="72"/>
-      <c r="D48" t="s">
+      <c r="B51" s="76"/>
+      <c r="C51" s="78"/>
+      <c r="D51" t="s">
         <v>100</v>
       </c>
-      <c r="G48" s="59" t="s">
+      <c r="G51" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="H48">
+      <c r="H51">
         <v>250000</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I51" t="s">
         <v>101</v>
       </c>
-      <c r="J48" s="46"/>
-      <c r="K48" s="46"/>
-      <c r="L48" s="46"/>
-      <c r="M48" s="46"/>
-      <c r="N48" s="46"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="75"/>
-      <c r="C49" s="72"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="59" t="s">
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="46"/>
+      <c r="M51" s="46"/>
+      <c r="N51" s="46"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B52" s="76"/>
+      <c r="C52" s="78"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="H49" s="19">
+      <c r="H52" s="19">
         <v>3300</v>
       </c>
-      <c r="I49" s="19" t="s">
+      <c r="I52" s="19" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="75"/>
-      <c r="C50" s="72"/>
-      <c r="G50" s="59" t="s">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B53" s="76"/>
+      <c r="C53" s="78"/>
+      <c r="G53" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="H50">
-        <f>H49/H46</f>
-        <v>3411.8995490946886</v>
-      </c>
-      <c r="I50" s="59" t="s">
+      <c r="H53" s="106">
+        <f>H52/H48</f>
+        <v>2629.1864160311047</v>
+      </c>
+      <c r="I53" s="59" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="75"/>
-      <c r="C51" s="72"/>
-      <c r="G51" s="59" t="s">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B54" s="76"/>
+      <c r="C54" s="78"/>
+      <c r="G54" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="H51" s="64">
-        <f>1/(2*PI()*H47*H50)</f>
-        <v>4.6647018999760829E-9</v>
-      </c>
-      <c r="I51" s="59" t="s">
+      <c r="H54" s="107">
+        <f>1/(2*PI()*H50*H53)</f>
+        <v>6.0533913503230433E-9</v>
+      </c>
+      <c r="I54" s="59" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="76"/>
-      <c r="C52" s="73"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="60" t="s">
+    <row r="55" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="103"/>
+      <c r="C55" s="79"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="H52" s="65">
-        <f>1/(2*PI()*H50*H48)</f>
-        <v>1.8658807599904334E-10</v>
-      </c>
-      <c r="I52" s="60" t="s">
+      <c r="H55" s="108">
+        <f>1/(2*PI()*H53*H51)</f>
+        <v>2.4213565401292174E-10</v>
+      </c>
+      <c r="I55" s="60" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="74" t="s">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B56" s="83" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="71" t="s">
+      <c r="C56" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="D53" s="68" t="s">
+      <c r="D56" s="102" t="s">
         <v>104</v>
       </c>
-      <c r="E53" s="68"/>
-      <c r="G53" s="59" t="s">
+      <c r="E56" s="102"/>
+      <c r="G56" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="H53">
+      <c r="H56">
         <f>(H3)/(2*PI()*120*H28*H4)</f>
         <v>3.2639197313767605</v>
       </c>
-      <c r="I53" s="59" t="s">
+      <c r="I56" s="59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="78"/>
-      <c r="C54" s="77"/>
-      <c r="G54" s="59" t="s">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B57" s="72"/>
+      <c r="C57" s="81"/>
+      <c r="G57" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="H54">
-        <f>H53*2</f>
+      <c r="H57">
+        <f>H56*2</f>
         <v>6.527839462753521</v>
       </c>
-      <c r="I54" s="59" t="s">
+      <c r="I57" s="59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="78"/>
-      <c r="C55" s="77"/>
-      <c r="G55" s="59" t="s">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B58" s="72"/>
+      <c r="C58" s="81"/>
+      <c r="G58" s="59" t="s">
         <v>116</v>
       </c>
-      <c r="H55">
+      <c r="H58">
         <f>0.075</f>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="I55" s="59" t="s">
+      <c r="I58" s="59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="78"/>
-      <c r="C56" s="77"/>
-      <c r="G56" s="59" t="s">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B59" s="72"/>
+      <c r="C59" s="81"/>
+      <c r="G59" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="H56">
-        <f>H55/H54</f>
+      <c r="H59">
+        <f>H58/H57</f>
         <v>1.1489253133128385E-2</v>
       </c>
-      <c r="I56" s="59" t="s">
+      <c r="I59" s="59" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="78"/>
-      <c r="C57" s="77"/>
-      <c r="G57" s="59" t="s">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B60" s="72"/>
+      <c r="C60" s="81"/>
+      <c r="G60" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="H57">
+      <c r="H60">
         <v>1360000</v>
       </c>
-      <c r="I57" s="59" t="s">
+      <c r="I60" s="59" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="78"/>
-      <c r="C58" s="77"/>
-      <c r="G58" s="59" t="s">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B61" s="72"/>
+      <c r="C61" s="81"/>
+      <c r="G61" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="H58">
+      <c r="H61">
         <v>11239</v>
       </c>
-      <c r="I58" s="59" t="s">
+      <c r="I61" s="59" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="78"/>
-      <c r="C59" s="77"/>
-      <c r="G59" s="59" t="s">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B62" s="72"/>
+      <c r="C62" s="81"/>
+      <c r="G62" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="H59" s="62">
-        <f>1/(2*PI()*120*H56*H57)</f>
+      <c r="H62" s="62">
+        <f>1/(2*PI()*120*H59*H60)</f>
         <v>8.4880548873167096E-8</v>
       </c>
-      <c r="I59" s="59" t="s">
+      <c r="I62" s="59" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" s="78"/>
-      <c r="C60" s="77"/>
-      <c r="G60" s="59" t="s">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B63" s="72"/>
+      <c r="C63" s="81"/>
+      <c r="G63" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="H60">
+      <c r="H63">
         <f xml:space="preserve"> H3/(2*PI()*H4*5*H28)</f>
         <v>78.334073553042259</v>
       </c>
-      <c r="I60" s="59"/>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="78"/>
-      <c r="C61" s="77"/>
-      <c r="G61" s="59" t="s">
+      <c r="I63" s="59"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B64" s="72"/>
+      <c r="C64" s="81"/>
+      <c r="G64" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="H61">
-        <f>1/(2*PI()*H57*H59)</f>
+      <c r="H64">
+        <f>1/(2*PI()*H60*H62)</f>
         <v>1.3787103759754062</v>
       </c>
-      <c r="I61" s="59"/>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="78"/>
-      <c r="C62" s="77"/>
-      <c r="G62" s="59" t="s">
+      <c r="I64" s="59"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="72"/>
+      <c r="C65" s="81"/>
+      <c r="G65" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="H62">
-        <f>SQRT(H60*H61)</f>
+      <c r="H65">
+        <f>SQRT(H63*H64)</f>
         <v>10.392304845413264</v>
       </c>
-      <c r="I62" s="59"/>
-    </row>
-    <row r="63" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="76"/>
-      <c r="C63" s="73"/>
-      <c r="D63" s="22"/>
-      <c r="E63" s="22"/>
-      <c r="F63" s="22"/>
-      <c r="G63" s="60" t="s">
+      <c r="I65" s="59"/>
+    </row>
+    <row r="66" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="103"/>
+      <c r="C66" s="79"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="H63" s="22">
-        <f>1/(2*PI()*H62*H59)</f>
+      <c r="H66" s="22">
+        <f>1/(2*PI()*H65*H62)</f>
         <v>180426.39618622433</v>
       </c>
-      <c r="I63" s="22"/>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B64">
+      <c r="I66" s="22"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67">
         <v>4.8</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C67" t="s">
         <v>121</v>
       </c>
-      <c r="H64">
+      <c r="H67">
         <f>7.5/H4</f>
         <v>2.1428571428571429E-2</v>
       </c>
-      <c r="I64">
-        <f>1/H64</f>
+      <c r="I67">
+        <f>1/H67</f>
         <v>46.666666666666664</v>
       </c>
     </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G65" t="s">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
         <v>122</v>
       </c>
-      <c r="H65">
+      <c r="H68">
         <v>2000000</v>
       </c>
     </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G66" t="s">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
         <v>123</v>
       </c>
-      <c r="H66">
-        <f>(H64)*H65*(1+(H64))</f>
+      <c r="H69">
+        <f>(H67)*H68*(1+(H67))</f>
         <v>43775.510204081627</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="J20:O20"/>
+    <mergeCell ref="J48:N48"/>
+    <mergeCell ref="C48:C55"/>
+    <mergeCell ref="B48:B55"/>
+    <mergeCell ref="J39:O39"/>
+    <mergeCell ref="C39:C45"/>
+    <mergeCell ref="B39:B45"/>
+    <mergeCell ref="J33:O33"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C56:C66"/>
+    <mergeCell ref="B56:B66"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="J25:O25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E7:F9"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J10:O12"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="J27:O27"/>
     <mergeCell ref="J24:O24"/>
@@ -5343,51 +5464,6 @@
     <mergeCell ref="C18:C22"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="J25:O25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E7:F9"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="J19:O19"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="J10:O12"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="J20:O20"/>
-    <mergeCell ref="J46:N46"/>
-    <mergeCell ref="C46:C52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="J39:O39"/>
-    <mergeCell ref="C39:C45"/>
-    <mergeCell ref="B39:B45"/>
-    <mergeCell ref="J33:O33"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="C53:C63"/>
-    <mergeCell ref="B53:B63"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J30" r:id="rId1" display="https://www.digikey.com/product-detail/en/cree-wolfspeed/C3D06065I/C3D06065I-ND/5067191"/>
@@ -5403,10 +5479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R17"/>
+  <dimension ref="A2:S17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5415,14 +5491,16 @@
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="84" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
       <c r="D2">
         <f>'Power Factor Correction'!H27</f>
         <v>1.1075596590909088E-4</v>
@@ -5431,113 +5509,163 @@
         <v>24</v>
       </c>
       <c r="M2" t="s">
+        <v>131</v>
+      </c>
+      <c r="N2" s="65" t="s">
         <v>132</v>
-      </c>
-      <c r="N2" s="67" t="s">
-        <v>133</v>
       </c>
       <c r="O2" t="s">
         <v>127</v>
       </c>
       <c r="P2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>140</v>
+      </c>
+      <c r="R2" t="s">
         <v>128</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>129</v>
       </c>
-      <c r="R2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="84" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
       <c r="D3">
-        <f>'Power Factor Correction'!H24</f>
-        <v>7.7059314853766185</v>
+        <f>'Power Factor Correction'!H24+('Power Factor Correction'!H24*0.2)</f>
+        <v>9.2471177824519426</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M3">
         <v>76</v>
       </c>
-      <c r="N3" s="67">
+      <c r="N3" s="65">
         <v>97</v>
       </c>
       <c r="O3">
-        <v>8.82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="P3">
+        <v>173</v>
+      </c>
+      <c r="Q3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M4">
         <v>360</v>
       </c>
-      <c r="N4" s="67">
+      <c r="N4" s="65">
         <v>360</v>
       </c>
       <c r="O4">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+      <c r="P4">
+        <v>340</v>
+      </c>
+      <c r="Q4">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M5">
         <v>124</v>
       </c>
-      <c r="N5" s="67">
+      <c r="N5" s="65">
         <v>153</v>
       </c>
       <c r="O5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+      <c r="P5">
+        <v>262</v>
+      </c>
+      <c r="Q5">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M6">
         <f>SQRT(D2/(M5*10^-9))</f>
         <v>29.886339244885953</v>
       </c>
-      <c r="N6" s="67">
+      <c r="N6" s="65">
         <f>SQRT($D$2/(N5*10^-9))</f>
         <v>26.905300630548652</v>
       </c>
-      <c r="O6" s="67">
-        <f>SQRT($D$2/(O5*10^-9))</f>
-        <v>33.280018916624861</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="O6" s="65">
+        <f t="shared" ref="O6:Q6" si="0">SQRT($D$2/(O5*10^-9))</f>
+        <v>23.771442083303473</v>
+      </c>
+      <c r="P6" s="65">
+        <f t="shared" si="0"/>
+        <v>20.560464350532239</v>
+      </c>
+      <c r="Q6" s="65">
+        <f t="shared" si="0"/>
+        <v>23.893661100143479</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M7">
         <f>($D$2*$D$3)/(ROUNDUP(M6,1)*M3*10^-6)</f>
-        <v>0.37558435349945551</v>
-      </c>
-      <c r="N7" s="67">
+        <v>0.45070122419934666</v>
+      </c>
+      <c r="N7" s="65">
         <f>($D$2*$D$3)/(ROUNDUP(N6,1)*N3*10^-6)</f>
-        <v>0.32587929930972231</v>
-      </c>
-      <c r="O7" s="67">
-        <f>($D$2*$D$3)/(ROUNDUP(O6,1)*O3*10^-6)</f>
-        <v>2.9058918949294958</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0.39105515917166683</v>
+      </c>
+      <c r="O7" s="65">
+        <f t="shared" ref="O7:Q7" si="1">($D$2*$D$3)/(ROUNDUP(O6,1)*O3*10^-6)</f>
+        <v>0.3442599871833934</v>
+      </c>
+      <c r="P7" s="65">
+        <f t="shared" si="1"/>
+        <v>0.28738241816897558</v>
+      </c>
+      <c r="Q7" s="65">
+        <f t="shared" si="1"/>
+        <v>0.24770200059752706</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>138</v>
+      </c>
+      <c r="P8">
+        <f>(P4*10^-3*ROUNDUP(P6,1)*P3*10^-6)/($D$2)</f>
+        <v>10.940196223782326</v>
+      </c>
+      <c r="Q8">
+        <f>(Q4*10^-3*ROUNDUP(Q6,1)*Q3*10^-6)/(D2)</f>
+        <v>12.692751929533864</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F16">
         <f>11.1*2*PI()*27</f>
         <v>1883.0706365617218</v>

</xml_diff>

<commit_message>
Working finished rev 2 of PCF PCB and creating BOMS
</commit_message>
<xml_diff>
--- a/Power Factor Correction/Design Files/UC2855A Calculations (Autosaved).xlsx
+++ b/Power Factor Correction/Design Files/UC2855A Calculations (Autosaved).xlsx
@@ -869,120 +869,120 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="167" fontId="6" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="6" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -4152,7 +4152,7 @@
   <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4197,14 +4197,14 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="84" t="s">
+      <c r="J3" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="84"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
@@ -4228,15 +4228,15 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="72">
+      <c r="B7" s="80">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="80" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
       <c r="G7" t="s">
         <v>1</v>
       </c>
@@ -4245,11 +4245,11 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
       <c r="G8" t="s">
         <v>58</v>
       </c>
@@ -4259,11 +4259,11 @@
       </c>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
       <c r="G9" s="16" t="s">
         <v>2</v>
       </c>
@@ -4272,18 +4272,18 @@
         <v>1.7857142857142858E-10</v>
       </c>
       <c r="I9" s="16"/>
-      <c r="J9" s="84" t="s">
+      <c r="J9" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="84"/>
-      <c r="N9" s="84"/>
-      <c r="O9" s="84"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="74"/>
     </row>
     <row r="10" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="47"/>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="107" t="s">
         <v>66</v>
       </c>
       <c r="D10" s="47" t="s">
@@ -4298,20 +4298,20 @@
       <c r="I10" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="91" t="s">
+      <c r="J10" s="73" t="s">
         <v>112</v>
       </c>
-      <c r="K10" s="91"/>
-      <c r="L10" s="91"/>
-      <c r="M10" s="91"/>
-      <c r="N10" s="91"/>
-      <c r="O10" s="91"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
     </row>
     <row r="11" spans="2:15" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="77">
+      <c r="B11" s="107">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C11" s="81"/>
+      <c r="C11" s="76"/>
       <c r="D11" s="14" t="s">
         <v>69</v>
       </c>
@@ -4324,16 +4324,16 @@
       <c r="I11" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="91"/>
-      <c r="K11" s="91"/>
-      <c r="L11" s="91"/>
-      <c r="M11" s="91"/>
-      <c r="N11" s="91"/>
-      <c r="O11" s="91"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="73"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="79"/>
-      <c r="C12" s="79"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
       <c r="D12" s="21" t="s">
         <v>111</v>
       </c>
@@ -4347,26 +4347,26 @@
       <c r="I12" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="91"/>
-      <c r="K12" s="91"/>
-      <c r="L12" s="91"/>
-      <c r="M12" s="91"/>
-      <c r="N12" s="91"/>
-      <c r="O12" s="91"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
     </row>
     <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="37">
         <v>3</v>
       </c>
-      <c r="C13" s="90" t="s">
+      <c r="C13" s="101" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90"/>
-      <c r="I13" s="90"/>
+      <c r="D13" s="101"/>
+      <c r="E13" s="101"/>
+      <c r="F13" s="101"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="101"/>
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
@@ -4395,10 +4395,10 @@
       <c r="O14" s="17"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="80" t="s">
+      <c r="C15" s="75" t="s">
         <v>76</v>
       </c>
       <c r="D15" s="39"/>
@@ -4419,8 +4419,8 @@
       <c r="O15" s="38"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="79"/>
-      <c r="C16" s="79"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
       <c r="D16" s="43" t="s">
         <v>79</v>
       </c>
@@ -4467,16 +4467,16 @@
       <c r="O17" s="38"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="80">
+      <c r="B18" s="75">
         <v>3.2</v>
       </c>
-      <c r="C18" s="80" t="s">
+      <c r="C18" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="83" t="s">
+      <c r="D18" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="E18" s="83"/>
+      <c r="E18" s="79"/>
       <c r="F18" s="48"/>
       <c r="G18" s="19"/>
       <c r="H18" s="34">
@@ -4493,9 +4493,9 @@
       <c r="O18" s="49"/>
     </row>
     <row r="19" spans="2:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="72" t="s">
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="80" t="s">
         <v>80</v>
       </c>
       <c r="E19" s="13"/>
@@ -4510,19 +4510,19 @@
       <c r="I19" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="J19" s="91" t="s">
+      <c r="J19" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="K19" s="91"/>
-      <c r="L19" s="91"/>
-      <c r="M19" s="91"/>
-      <c r="N19" s="91"/>
-      <c r="O19" s="91"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="73"/>
+      <c r="N19" s="73"/>
+      <c r="O19" s="73"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="72"/>
+      <c r="B20" s="76"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="80"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="19"/>
@@ -4533,18 +4533,18 @@
       <c r="I20" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="91" t="s">
+      <c r="J20" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="K20" s="91"/>
-      <c r="L20" s="91"/>
-      <c r="M20" s="91"/>
-      <c r="N20" s="91"/>
-      <c r="O20" s="91"/>
+      <c r="K20" s="73"/>
+      <c r="L20" s="73"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="73"/>
+      <c r="O20" s="73"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="76"/>
       <c r="D21" s="39" t="s">
         <v>84</v>
       </c>
@@ -4567,8 +4567,8 @@
       <c r="O21" s="38"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="82"/>
-      <c r="C22" s="82"/>
+      <c r="B22" s="108"/>
+      <c r="C22" s="108"/>
       <c r="D22" s="14" t="s">
         <v>83</v>
       </c>
@@ -4589,28 +4589,28 @@
       <c r="B23" s="3">
         <v>4.2</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="105"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="105"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="2:15" ht="53.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="77" t="s">
+      <c r="C24" s="107" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="85"/>
-      <c r="F24" s="85"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
       <c r="G24" s="4" t="s">
         <v>13</v>
       </c>
@@ -4621,23 +4621,23 @@
       <c r="I24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J24" s="71" t="s">
+      <c r="J24" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="K24" s="71"/>
-      <c r="L24" s="71"/>
-      <c r="M24" s="71"/>
-      <c r="N24" s="71"/>
-      <c r="O24" s="71"/>
+      <c r="K24" s="104"/>
+      <c r="L24" s="104"/>
+      <c r="M24" s="104"/>
+      <c r="N24" s="104"/>
+      <c r="O24" s="104"/>
     </row>
     <row r="25" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="76"/>
-      <c r="C25" s="78"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="77"/>
       <c r="D25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
       <c r="G25" s="5" t="s">
         <v>16</v>
       </c>
@@ -4648,21 +4648,21 @@
       <c r="I25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J25" s="87" t="s">
+      <c r="J25" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="87"/>
-      <c r="N25" s="87"/>
-      <c r="O25" s="87"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
+      <c r="N25" s="100"/>
+      <c r="O25" s="100"/>
     </row>
     <row r="26" spans="2:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D26" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="84"/>
       <c r="G26" s="10" t="s">
         <v>21</v>
       </c>
@@ -4684,8 +4684,8 @@
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
+      <c r="E27" s="102"/>
+      <c r="F27" s="102"/>
       <c r="G27" s="21" t="s">
         <v>23</v>
       </c>
@@ -4696,12 +4696,12 @@
       <c r="I27" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="70"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="70"/>
-      <c r="M27" s="70"/>
-      <c r="N27" s="70"/>
-      <c r="O27" s="70"/>
+      <c r="J27" s="103"/>
+      <c r="K27" s="103"/>
+      <c r="L27" s="103"/>
+      <c r="M27" s="103"/>
+      <c r="N27" s="103"/>
+      <c r="O27" s="103"/>
     </row>
     <row r="28" spans="2:15" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
@@ -4713,8 +4713,8 @@
       <c r="D28" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="92"/>
-      <c r="F28" s="92"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="94"/>
       <c r="G28" s="23" t="s">
         <v>28</v>
       </c>
@@ -4723,75 +4723,75 @@
         <v>5.1083900226757363E-4</v>
       </c>
       <c r="I28" s="25"/>
-      <c r="J28" s="96" t="s">
+      <c r="J28" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="K28" s="96"/>
-      <c r="L28" s="96"/>
-      <c r="M28" s="96"/>
-      <c r="N28" s="96"/>
+      <c r="K28" s="98"/>
+      <c r="L28" s="98"/>
+      <c r="M28" s="98"/>
+      <c r="N28" s="98"/>
     </row>
     <row r="29" spans="2:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="72" t="s">
+      <c r="B29" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="81" t="s">
+      <c r="C29" s="76" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="93" t="s">
+      <c r="E29" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="93"/>
-      <c r="G29" s="93"/>
-      <c r="H29" s="93"/>
+      <c r="F29" s="95"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="95"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="94" t="s">
+      <c r="J29" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="K29" s="94"/>
+      <c r="K29" s="96"/>
       <c r="L29" t="s">
         <v>33</v>
       </c>
-      <c r="M29" s="94" t="s">
+      <c r="M29" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="N29" s="94"/>
+      <c r="N29" s="96"/>
     </row>
     <row r="30" spans="2:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="72"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="99" t="s">
+      <c r="B30" s="80"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="95" t="s">
+      <c r="E30" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="95"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="95"/>
-      <c r="J30" s="94" t="s">
+      <c r="F30" s="97"/>
+      <c r="G30" s="97"/>
+      <c r="H30" s="97"/>
+      <c r="J30" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="K30" s="94"/>
+      <c r="K30" s="96"/>
       <c r="L30" t="s">
         <v>33</v>
       </c>
-      <c r="M30" s="94" t="s">
+      <c r="M30" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="N30" s="94"/>
+      <c r="N30" s="96"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="73"/>
-      <c r="C31" s="101"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="89" t="s">
+      <c r="B31" s="92"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="89"/>
+      <c r="F31" s="93"/>
       <c r="G31" s="20" t="s">
         <v>38</v>
       </c>
@@ -4806,28 +4806,28 @@
       <c r="B32" s="27">
         <v>4.3</v>
       </c>
-      <c r="C32" s="97" t="s">
+      <c r="C32" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="97"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="97"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="97"/>
-      <c r="I32" s="97"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="87"/>
     </row>
     <row r="33" spans="2:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="83" t="s">
+      <c r="B33" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="80" t="s">
+      <c r="C33" s="75" t="s">
         <v>42</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E33" s="98"/>
-      <c r="F33" s="98"/>
+      <c r="E33" s="88"/>
+      <c r="F33" s="88"/>
       <c r="G33" s="28" t="s">
         <v>47</v>
       </c>
@@ -4838,23 +4838,23 @@
       <c r="I33" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="J33" s="104" t="s">
+      <c r="J33" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="K33" s="104"/>
-      <c r="L33" s="104"/>
-      <c r="M33" s="104"/>
-      <c r="N33" s="104"/>
-      <c r="O33" s="104"/>
+      <c r="K33" s="83"/>
+      <c r="L33" s="83"/>
+      <c r="M33" s="83"/>
+      <c r="N33" s="83"/>
+      <c r="O33" s="83"/>
     </row>
     <row r="34" spans="2:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="72"/>
-      <c r="C34" s="81"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="76"/>
       <c r="D34" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="86"/>
-      <c r="F34" s="86"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="84"/>
       <c r="G34" s="11" t="s">
         <v>46</v>
       </c>
@@ -4867,13 +4867,13 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="72"/>
-      <c r="C35" s="81"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="76"/>
       <c r="D35" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="84"/>
       <c r="G35" s="11" t="s">
         <v>45</v>
       </c>
@@ -4886,13 +4886,13 @@
       </c>
     </row>
     <row r="36" spans="2:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="72"/>
-      <c r="C36" s="81"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="76"/>
       <c r="D36" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
+      <c r="E36" s="84"/>
+      <c r="F36" s="84"/>
       <c r="G36" s="11"/>
       <c r="H36" s="11">
         <f>SQRT(H35/(H39*10^-12))</f>
@@ -4901,13 +4901,13 @@
       <c r="I36" s="11"/>
     </row>
     <row r="37" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="72"/>
-      <c r="C37" s="81"/>
+      <c r="B37" s="80"/>
+      <c r="C37" s="76"/>
       <c r="D37" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
+      <c r="E37" s="84"/>
+      <c r="F37" s="84"/>
       <c r="G37" s="11"/>
       <c r="H37" s="11">
         <f>SQRT(1/(H35*(H39*10^-12)))</f>
@@ -4916,13 +4916,13 @@
       <c r="I37" s="11"/>
     </row>
     <row r="38" spans="2:15" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="103"/>
-      <c r="C38" s="79"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="78"/>
       <c r="D38" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="88"/>
-      <c r="F38" s="105"/>
+      <c r="E38" s="85"/>
+      <c r="F38" s="86"/>
       <c r="G38" s="22"/>
       <c r="H38" s="22">
         <f>H24+(H4/H36)</f>
@@ -4931,10 +4931,10 @@
       <c r="I38" s="22"/>
     </row>
     <row r="39" spans="2:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="83" t="s">
+      <c r="B39" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="80" t="s">
+      <c r="C39" s="75" t="s">
         <v>65</v>
       </c>
       <c r="D39" s="32" t="s">
@@ -4950,18 +4950,18 @@
       <c r="I39" t="s">
         <v>53</v>
       </c>
-      <c r="J39" s="91" t="s">
+      <c r="J39" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="K39" s="91"/>
-      <c r="L39" s="91"/>
-      <c r="M39" s="91"/>
-      <c r="N39" s="91"/>
-      <c r="O39" s="91"/>
+      <c r="K39" s="73"/>
+      <c r="L39" s="73"/>
+      <c r="M39" s="73"/>
+      <c r="N39" s="73"/>
+      <c r="O39" s="73"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="72"/>
-      <c r="C40" s="81"/>
+      <c r="B40" s="80"/>
+      <c r="C40" s="76"/>
       <c r="G40" t="s">
         <v>57</v>
       </c>
@@ -4974,8 +4974,8 @@
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="72"/>
-      <c r="C41" s="81"/>
+      <c r="B41" s="80"/>
+      <c r="C41" s="76"/>
       <c r="G41" t="s">
         <v>56</v>
       </c>
@@ -4988,8 +4988,8 @@
       </c>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="72"/>
-      <c r="C42" s="81"/>
+      <c r="B42" s="80"/>
+      <c r="C42" s="76"/>
       <c r="G42" t="s">
         <v>59</v>
       </c>
@@ -4999,8 +4999,8 @@
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="72"/>
-      <c r="C43" s="81"/>
+      <c r="B43" s="80"/>
+      <c r="C43" s="76"/>
       <c r="G43" t="s">
         <v>61</v>
       </c>
@@ -5013,8 +5013,8 @@
       </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="72"/>
-      <c r="C44" s="81"/>
+      <c r="B44" s="80"/>
+      <c r="C44" s="76"/>
       <c r="G44" t="s">
         <v>62</v>
       </c>
@@ -5027,8 +5027,8 @@
       </c>
     </row>
     <row r="45" spans="2:15" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="103"/>
-      <c r="C45" s="79"/>
+      <c r="B45" s="82"/>
+      <c r="C45" s="78"/>
       <c r="D45" s="42" t="s">
         <v>64</v>
       </c>
@@ -5070,10 +5070,10 @@
       <c r="I47" s="19"/>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="83" t="s">
+      <c r="B48" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="C48" s="80" t="s">
+      <c r="C48" s="75" t="s">
         <v>98</v>
       </c>
       <c r="D48" t="s">
@@ -5086,17 +5086,17 @@
         <f>(H4*((1/H18)*H19)/((2*PI()*H50*H27*5.2)))</f>
         <v>1.2551411265016057</v>
       </c>
-      <c r="J48" s="84" t="s">
+      <c r="J48" s="74" t="s">
         <v>90</v>
       </c>
-      <c r="K48" s="84"/>
-      <c r="L48" s="84"/>
-      <c r="M48" s="84"/>
-      <c r="N48" s="84"/>
+      <c r="K48" s="74"/>
+      <c r="L48" s="74"/>
+      <c r="M48" s="74"/>
+      <c r="N48" s="74"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B49" s="72"/>
-      <c r="C49" s="81"/>
+      <c r="B49" s="80"/>
+      <c r="C49" s="76"/>
       <c r="G49" s="59" t="s">
         <v>141</v>
       </c>
@@ -5111,8 +5111,8 @@
       <c r="N49" s="66"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B50" s="76"/>
-      <c r="C50" s="78"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="77"/>
       <c r="D50" t="s">
         <v>99</v>
       </c>
@@ -5135,8 +5135,8 @@
       <c r="A51" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="76"/>
-      <c r="C51" s="78"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="77"/>
       <c r="D51" t="s">
         <v>100</v>
       </c>
@@ -5156,8 +5156,8 @@
       <c r="N51" s="46"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B52" s="76"/>
-      <c r="C52" s="78"/>
+      <c r="B52" s="81"/>
+      <c r="C52" s="77"/>
       <c r="D52" s="19"/>
       <c r="E52" s="19"/>
       <c r="F52" s="19"/>
@@ -5172,12 +5172,12 @@
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B53" s="76"/>
-      <c r="C53" s="78"/>
+      <c r="B53" s="81"/>
+      <c r="C53" s="77"/>
       <c r="G53" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="H53" s="106">
+      <c r="H53" s="69">
         <f>H52/H48</f>
         <v>2629.1864160311047</v>
       </c>
@@ -5186,12 +5186,12 @@
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B54" s="76"/>
-      <c r="C54" s="78"/>
+      <c r="B54" s="81"/>
+      <c r="C54" s="77"/>
       <c r="G54" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="H54" s="107">
+      <c r="H54" s="70">
         <f>1/(2*PI()*H50*H53)</f>
         <v>6.0533913503230433E-9</v>
       </c>
@@ -5200,15 +5200,15 @@
       </c>
     </row>
     <row r="55" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="103"/>
-      <c r="C55" s="79"/>
+      <c r="B55" s="82"/>
+      <c r="C55" s="78"/>
       <c r="D55" s="22"/>
       <c r="E55" s="22"/>
       <c r="F55" s="22"/>
       <c r="G55" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="H55" s="108">
+      <c r="H55" s="71">
         <f>1/(2*PI()*H53*H51)</f>
         <v>2.4213565401292174E-10</v>
       </c>
@@ -5217,16 +5217,16 @@
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B56" s="83" t="s">
+      <c r="B56" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="C56" s="80" t="s">
+      <c r="C56" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="D56" s="102" t="s">
+      <c r="D56" s="72" t="s">
         <v>104</v>
       </c>
-      <c r="E56" s="102"/>
+      <c r="E56" s="72"/>
       <c r="G56" s="59" t="s">
         <v>103</v>
       </c>
@@ -5239,8 +5239,8 @@
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B57" s="72"/>
-      <c r="C57" s="81"/>
+      <c r="B57" s="80"/>
+      <c r="C57" s="76"/>
       <c r="G57" s="59" t="s">
         <v>105</v>
       </c>
@@ -5253,8 +5253,8 @@
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B58" s="72"/>
-      <c r="C58" s="81"/>
+      <c r="B58" s="80"/>
+      <c r="C58" s="76"/>
       <c r="G58" s="59" t="s">
         <v>116</v>
       </c>
@@ -5267,8 +5267,8 @@
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B59" s="72"/>
-      <c r="C59" s="81"/>
+      <c r="B59" s="80"/>
+      <c r="C59" s="76"/>
       <c r="G59" s="59" t="s">
         <v>117</v>
       </c>
@@ -5281,8 +5281,8 @@
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B60" s="72"/>
-      <c r="C60" s="81"/>
+      <c r="B60" s="80"/>
+      <c r="C60" s="76"/>
       <c r="G60" s="59" t="s">
         <v>106</v>
       </c>
@@ -5294,8 +5294,8 @@
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B61" s="72"/>
-      <c r="C61" s="81"/>
+      <c r="B61" s="80"/>
+      <c r="C61" s="76"/>
       <c r="G61" s="59" t="s">
         <v>107</v>
       </c>
@@ -5307,8 +5307,8 @@
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B62" s="72"/>
-      <c r="C62" s="81"/>
+      <c r="B62" s="80"/>
+      <c r="C62" s="76"/>
       <c r="G62" s="59" t="s">
         <v>108</v>
       </c>
@@ -5321,8 +5321,8 @@
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B63" s="72"/>
-      <c r="C63" s="81"/>
+      <c r="B63" s="80"/>
+      <c r="C63" s="76"/>
       <c r="G63" s="59" t="s">
         <v>118</v>
       </c>
@@ -5333,8 +5333,8 @@
       <c r="I63" s="59"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B64" s="72"/>
-      <c r="C64" s="81"/>
+      <c r="B64" s="80"/>
+      <c r="C64" s="76"/>
       <c r="G64" s="59" t="s">
         <v>120</v>
       </c>
@@ -5345,8 +5345,8 @@
       <c r="I64" s="59"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B65" s="72"/>
-      <c r="C65" s="81"/>
+      <c r="B65" s="80"/>
+      <c r="C65" s="76"/>
       <c r="G65" s="59" t="s">
         <v>119</v>
       </c>
@@ -5357,8 +5357,8 @@
       <c r="I65" s="59"/>
     </row>
     <row r="66" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="103"/>
-      <c r="C66" s="79"/>
+      <c r="B66" s="82"/>
+      <c r="C66" s="78"/>
       <c r="D66" s="22"/>
       <c r="E66" s="22"/>
       <c r="F66" s="22"/>
@@ -5406,6 +5406,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="J27:O27"/>
+    <mergeCell ref="J24:O24"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="J25:O25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E7:F9"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="J19:O19"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="J9:O9"/>
+    <mergeCell ref="J10:O12"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="C32:I32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C29:C31"/>
     <mergeCell ref="D56:E56"/>
     <mergeCell ref="J20:O20"/>
     <mergeCell ref="J48:N48"/>
@@ -5422,48 +5464,6 @@
     <mergeCell ref="B33:B38"/>
     <mergeCell ref="C56:C66"/>
     <mergeCell ref="B56:B66"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="J25:O25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E7:F9"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="J19:O19"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="J9:O9"/>
-    <mergeCell ref="J10:O12"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="J27:O27"/>
-    <mergeCell ref="J24:O24"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="D18:E18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J30" r:id="rId1" display="https://www.digikey.com/product-detail/en/cree-wolfspeed/C3D06065I/C3D06065I-ND/5067191"/>
@@ -5496,11 +5496,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="74" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
       <c r="D2">
         <f>'Power Factor Correction'!H27</f>
         <v>1.1075596590909088E-4</v>
@@ -5531,11 +5531,11 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
       <c r="D3">
         <f>'Power Factor Correction'!H24+('Power Factor Correction'!H24*0.2)</f>
         <v>9.2471177824519426</v>

</xml_diff>